<commit_message>
Moved all the inherent plant properties to PlantProperties. Started work on seeds.
</commit_message>
<xml_diff>
--- a/Design docs/sunlightstats.xlsx
+++ b/Design docs/sunlightstats.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="150">
   <si>
     <t>01월</t>
   </si>
@@ -519,6 +519,26 @@
     <t>night length</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>max</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>min</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>night length</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>day length</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -813,94 +833,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>34.127120692428996</c:v>
+                  <c:v>32.368701656654501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.84971330607528</c:v>
+                  <c:v>29.391405596902064</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.89434473575859</c:v>
+                  <c:v>27.861720334803287</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.831198074135095</c:v>
+                  <c:v>30.117052544330104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.649502373689785</c:v>
+                  <c:v>26.715127698019575</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.716359812581729</c:v>
+                  <c:v>26.479623961825599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.032080317391458</c:v>
+                  <c:v>27.861775571505913</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.735661403859748</c:v>
+                  <c:v>25.797220892258956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.322341962945035</c:v>
+                  <c:v>28.777528933931428</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28.316183166790104</c:v>
+                  <c:v>28.728274830813668</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.5808308589374</c:v>
+                  <c:v>28.028725245682764</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.158890128296058</c:v>
+                  <c:v>31.510592966679489</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.036924733397072</c:v>
+                  <c:v>25.738951092309932</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.734976051303434</c:v>
+                  <c:v>26.72990000334017</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.277119828130864</c:v>
+                  <c:v>29.131910034835961</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.2788593050552</c:v>
+                  <c:v>22.258885185989509</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.930090873907702</c:v>
+                  <c:v>24.483574418736488</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.379903688760344</c:v>
+                  <c:v>24.772246623600882</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.356627209704243</c:v>
+                  <c:v>23.796853464006148</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23.765302085637547</c:v>
+                  <c:v>28.497969671744329</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.88917003853819</c:v>
+                  <c:v>22.984643637378198</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22.223356965714082</c:v>
+                  <c:v>26.583663721800033</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>24.046598217206618</c:v>
+                  <c:v>27.592032909420816</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20.412938583240152</c:v>
+                  <c:v>31.589558455713629</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.834656815081075</c:v>
+                  <c:v>22.351033984166872</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24.958554145566019</c:v>
+                  <c:v>23.234465344419277</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>24.184791506035069</c:v>
+                  <c:v>24.469177758229122</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>25.267858324675117</c:v>
+                  <c:v>26.189185823743802</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>25.496578603723439</c:v>
+                  <c:v>28.560428850190661</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>26.555095000924386</c:v>
+                  <c:v>21.975693669987223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -936,94 +956,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>21.519469376384738</c:v>
+                  <c:v>25.215260395062391</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.074343764678261</c:v>
+                  <c:v>22.145668079642252</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.760772854001502</c:v>
+                  <c:v>18.359330345228397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.505671474286657</c:v>
+                  <c:v>18.269011418315554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.570379825936332</c:v>
+                  <c:v>23.520157241313434</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.872094893808288</c:v>
+                  <c:v>22.933491370605889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.543411204881259</c:v>
+                  <c:v>17.338926267049509</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.474669220972544</c:v>
+                  <c:v>16.784268409265042</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.053235003050077</c:v>
+                  <c:v>18.802611478000724</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23.167308624116618</c:v>
+                  <c:v>21.187910772477252</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24.655076988772485</c:v>
+                  <c:v>20.509306205081604</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.003146152757608</c:v>
+                  <c:v>17.257214847628202</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.800721269909211</c:v>
+                  <c:v>16.7947763832777</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.47555573541765</c:v>
+                  <c:v>18.771918912222858</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.68161513391777</c:v>
+                  <c:v>16.647184988744243</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.512459153581155</c:v>
+                  <c:v>16.326498623696317</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.726509238935968</c:v>
+                  <c:v>14.790588376920999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.400273049616196</c:v>
+                  <c:v>13.647592625090283</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.504728007808851</c:v>
+                  <c:v>13.517109086458346</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21.205693042252619</c:v>
+                  <c:v>18.717095203175752</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.182544901829324</c:v>
+                  <c:v>18.524278372461524</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14.487811051584201</c:v>
+                  <c:v>20.71529030284762</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.578928657385088</c:v>
+                  <c:v>19.474879279340399</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18.178854522817993</c:v>
+                  <c:v>12.774441542397964</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>21.310738945384273</c:v>
+                  <c:v>16.201720618556866</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17.464349368681553</c:v>
+                  <c:v>12.634186534345524</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17.147833977484773</c:v>
+                  <c:v>15.112027072439044</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.196004409124351</c:v>
+                  <c:v>10.996984679591822</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>16.597882564959697</c:v>
+                  <c:v>14.728821539318091</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.695562075582753</c:v>
+                  <c:v>8.7474648244060909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1040,11 +1060,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="177101312"/>
-        <c:axId val="76131712"/>
+        <c:axId val="184179200"/>
+        <c:axId val="166497088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="177101312"/>
+        <c:axId val="184179200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1073,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76131712"/>
+        <c:crossAx val="166497088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1061,7 +1081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76131712"/>
+        <c:axId val="166497088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1111,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177101312"/>
+        <c:crossAx val="184179200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1378,11 +1398,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="183676928"/>
-        <c:axId val="76134016"/>
+        <c:axId val="184463360"/>
+        <c:axId val="166499392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="183676928"/>
+        <c:axId val="184463360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,7 +1411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76134016"/>
+        <c:crossAx val="166499392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1399,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76134016"/>
+        <c:axId val="166499392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,7 +1430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183676928"/>
+        <c:crossAx val="184463360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1464,94 +1484,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>111.26208975111179</c:v>
+                  <c:v>111.84024915523568</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107.76564414323201</c:v>
+                  <c:v>54.847910366204488</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108.90893395225127</c:v>
+                  <c:v>109.74333356427809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.021204965562973</c:v>
+                  <c:v>110.41095666046003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.71480772046159</c:v>
+                  <c:v>103.66801115994332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.24218588728667</c:v>
+                  <c:v>49.628544443785216</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47.266088756857634</c:v>
+                  <c:v>94.948822284544448</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.220550422967122</c:v>
+                  <c:v>89.069305904418229</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43.59402671988731</c:v>
+                  <c:v>87.235359291730873</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86.498022909629555</c:v>
+                  <c:v>86.223633624579534</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.616429143793454</c:v>
+                  <c:v>85.459533230531918</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>86.713639528818405</c:v>
+                  <c:v>86.516150103653771</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43.139874757613477</c:v>
+                  <c:v>86.595876739797902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45.482341136398887</c:v>
+                  <c:v>90.375259727370832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>91.298168066749824</c:v>
+                  <c:v>90.519681934767718</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.03016560939686</c:v>
+                  <c:v>46.038648974559322</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>88.247577041710784</c:v>
+                  <c:v>43.536833332364289</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>94.746479047444765</c:v>
+                  <c:v>95.297216806581318</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>91.334019052255726</c:v>
+                  <c:v>45.297975968785927</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>47.410650245309242</c:v>
+                  <c:v>94.12221143173619</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>46.005990561643841</c:v>
+                  <c:v>45.875949719701822</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>46.678731479532644</c:v>
+                  <c:v>92.607262176590794</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>47.735273510810565</c:v>
+                  <c:v>94.207115903211161</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>92.793250186515706</c:v>
+                  <c:v>91.935005122360849</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44.139522966515806</c:v>
+                  <c:v>44.192833903096769</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>90.370756735941782</c:v>
+                  <c:v>44.911533440695862</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>90.577495052639293</c:v>
+                  <c:v>91.076865674527227</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>86.355441310054687</c:v>
+                  <c:v>86.460776735612825</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>88.70356188739342</c:v>
+                  <c:v>88.757132702114163</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>88.465179612272934</c:v>
+                  <c:v>89.294092413167022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1571,94 +1591,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>111.26208975111179</c:v>
+                  <c:v>111.84024915523568</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107.76564414323201</c:v>
+                  <c:v>65.614875072086846</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108.90893395225127</c:v>
+                  <c:v>109.74333356427809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.977063789092384</c:v>
+                  <c:v>110.41095666046003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.71480772046159</c:v>
+                  <c:v>103.66801115994332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.24218588728667</c:v>
+                  <c:v>59.639932679079337</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.710794639210576</c:v>
+                  <c:v>94.948822284544448</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.220550422967122</c:v>
+                  <c:v>89.069305904418229</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.283156131652021</c:v>
+                  <c:v>87.235359291730873</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86.498022909629555</c:v>
+                  <c:v>86.223633624579534</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.616429143793454</c:v>
+                  <c:v>85.459533230531918</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>86.713639528818405</c:v>
+                  <c:v>86.516150103653771</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51.82900416937818</c:v>
+                  <c:v>86.595876739797902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54.549258783457709</c:v>
+                  <c:v>90.375259727370832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>91.298168066749824</c:v>
+                  <c:v>90.519681934767718</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.03016560939686</c:v>
+                  <c:v>55.294460739265205</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>88.247577041710784</c:v>
+                  <c:v>52.414856861776059</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>94.746479047444765</c:v>
+                  <c:v>95.297216806581318</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>91.334019052255726</c:v>
+                  <c:v>54.36489361584475</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>56.855356127662183</c:v>
+                  <c:v>94.12221143173619</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>55.261802326349724</c:v>
+                  <c:v>55.131761484407704</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>55.934543244238526</c:v>
+                  <c:v>92.607262176590794</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>57.179979393163507</c:v>
+                  <c:v>94.207115903211161</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>92.793250186515706</c:v>
+                  <c:v>91.935005122360849</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53.017546495927576</c:v>
+                  <c:v>53.070857432508532</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>90.370756735941782</c:v>
+                  <c:v>53.978451087754685</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>90.577495052639293</c:v>
+                  <c:v>91.076865674527227</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>86.355441310054687</c:v>
+                  <c:v>86.460776735612825</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>88.70356188739342</c:v>
+                  <c:v>88.757132702114163</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>88.465179612272934</c:v>
+                  <c:v>89.294092413167022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1675,11 +1695,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="183678464"/>
-        <c:axId val="76135744"/>
+        <c:axId val="184464896"/>
+        <c:axId val="166501120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="183678464"/>
+        <c:axId val="184464896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76135744"/>
+        <c:crossAx val="166501120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1696,7 +1716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76135744"/>
+        <c:axId val="166501120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,7 +1727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183678464"/>
+        <c:crossAx val="184464896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2875,11 +2895,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="183678976"/>
-        <c:axId val="191374464"/>
+        <c:axId val="184465408"/>
+        <c:axId val="191242816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="183678976"/>
+        <c:axId val="184465408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2888,7 +2908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191374464"/>
+        <c:crossAx val="191242816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2896,7 +2916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191374464"/>
+        <c:axId val="191242816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2907,7 +2927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183678976"/>
+        <c:crossAx val="184465408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4051,8 +4071,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="183680512"/>
-        <c:axId val="191376192"/>
+        <c:axId val="184466944"/>
+        <c:axId val="191244544"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6259,11 +6279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190259712"/>
-        <c:axId val="191376768"/>
+        <c:axId val="191119872"/>
+        <c:axId val="191245120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="183680512"/>
+        <c:axId val="184466944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6272,7 +6292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191376192"/>
+        <c:crossAx val="191244544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6280,7 +6300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191376192"/>
+        <c:axId val="191244544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6291,12 +6311,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183680512"/>
+        <c:crossAx val="184466944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191376768"/>
+        <c:axId val="191245120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6306,12 +6326,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190259712"/>
+        <c:crossAx val="191119872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="190259712"/>
+        <c:axId val="191119872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6320,7 +6340,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191376768"/>
+        <c:crossAx val="191245120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7500,8 +7520,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190261760"/>
-        <c:axId val="191379648"/>
+        <c:axId val="191121920"/>
+        <c:axId val="191248000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9768,11 +9788,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190260736"/>
-        <c:axId val="191379072"/>
+        <c:axId val="191120896"/>
+        <c:axId val="191247424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190260736"/>
+        <c:axId val="191120896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9781,7 +9801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191379072"/>
+        <c:crossAx val="191247424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9789,7 +9809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191379072"/>
+        <c:axId val="191247424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9800,12 +9820,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190260736"/>
+        <c:crossAx val="191120896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191379648"/>
+        <c:axId val="191248000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9815,12 +9835,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190261760"/>
+        <c:crossAx val="191121920"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="190261760"/>
+        <c:axId val="191121920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9829,7 +9849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191379648"/>
+        <c:crossAx val="191248000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11015,11 +11035,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190262272"/>
-        <c:axId val="190415424"/>
+        <c:axId val="191122432"/>
+        <c:axId val="191594496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190262272"/>
+        <c:axId val="191122432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11028,7 +11048,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190415424"/>
+        <c:crossAx val="191594496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11036,7 +11056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190415424"/>
+        <c:axId val="191594496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11047,7 +11067,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190262272"/>
+        <c:crossAx val="191122432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13323,8 +13343,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190417152"/>
-        <c:axId val="190417728"/>
+        <c:axId val="191596224"/>
+        <c:axId val="191596800"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -15564,11 +15584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190418880"/>
-        <c:axId val="190418304"/>
+        <c:axId val="191597952"/>
+        <c:axId val="191597376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190417152"/>
+        <c:axId val="191596224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15578,12 +15598,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190417728"/>
+        <c:crossAx val="191596800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190417728"/>
+        <c:axId val="191596800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15594,12 +15614,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190417152"/>
+        <c:crossAx val="191596224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190418304"/>
+        <c:axId val="191597376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15609,12 +15629,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190418880"/>
+        <c:crossAx val="191597952"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190418880"/>
+        <c:axId val="191597952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15624,7 +15644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190418304"/>
+        <c:crossAx val="191597376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15873,15 +15893,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>280986</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>595313</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20196,35 +20216,35 @@
       </c>
       <c r="L3">
         <f ca="1">_xlfn.NORM.INV(RAND(), IF(K3=1,E3,F3), $B$35)</f>
-        <v>34.127120692428996</v>
+        <v>32.368701656654501</v>
       </c>
       <c r="M3">
         <f ca="1">_xlfn.NORM.INV(RAND(), G3, $C$35/3)</f>
-        <v>21.519469376384738</v>
+        <v>25.215260395062391</v>
       </c>
       <c r="N3">
         <f ca="1">L3</f>
-        <v>34.127120692428996</v>
+        <v>32.368701656654501</v>
       </c>
       <c r="O3">
         <f ca="1">_xlfn.NORM.INV(RAND(), IF(K3=1,J3,I3), $D$35)</f>
-        <v>111.26208975111179</v>
+        <v>111.84024915523568</v>
       </c>
       <c r="P3">
         <f ca="1">IF(K3=1, O3 + 0.1 * I3, O3)</f>
-        <v>111.26208975111179</v>
+        <v>111.84024915523568</v>
       </c>
       <c r="Q3">
         <f ca="1">IF(N3 &lt; M3, M3, N3)</f>
-        <v>34.127120692428996</v>
+        <v>32.368701656654501</v>
       </c>
       <c r="R3">
         <f ca="1">IF(N3 &lt; M3, N3, M3)</f>
-        <v>21.519469376384738</v>
+        <v>25.215260395062391</v>
       </c>
       <c r="S3">
         <f ca="1">AVERAGE(Q3,R3)</f>
-        <v>27.823295034406868</v>
+        <v>28.791981025858448</v>
       </c>
       <c r="AB3">
         <v>12.581799999999999</v>
@@ -20272,39 +20292,39 @@
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L32" ca="1" si="7">_xlfn.NORM.INV(RAND(), IF(K4=1,E4,F4), $B$35)</f>
-        <v>26.280361459486848</v>
+        <v>28.647081581963953</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M32" ca="1" si="8">_xlfn.NORM.INV(RAND(), G4, $C$35/3)</f>
-        <v>21.074343764678261</v>
+        <v>22.145668079642252</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N32" ca="1" si="9">N3 * $N$1 + (1-$N$1) * L4</f>
-        <v>27.84971330607528</v>
+        <v>29.391405596902064</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O32" ca="1" si="10">_xlfn.NORM.INV(RAND(), IF(K4=1,J4,I4), $D$35)</f>
-        <v>107.76564414323201</v>
+        <v>54.847910366204488</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P32" ca="1" si="11">IF(K4=1, O4 + 0.1 * I4, O4)</f>
-        <v>107.76564414323201</v>
+        <v>65.614875072086846</v>
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q32" ca="1" si="12">IF(N4 &lt; M4, M4, N4)</f>
-        <v>27.84971330607528</v>
+        <v>29.391405596902064</v>
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R32" ca="1" si="13">IF(N4 &lt; M4, N4, M4)</f>
-        <v>21.074343764678261</v>
+        <v>22.145668079642252</v>
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S32" ca="1" si="14">AVERAGE(Q4,R4)</f>
-        <v>24.462028535376771</v>
+        <v>25.768536838272158</v>
       </c>
       <c r="AB4">
         <v>8.5861499999999999</v>
@@ -20356,35 +20376,35 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="7"/>
-        <v>31.655502593179417</v>
+        <v>27.479299019278589</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="8"/>
-        <v>19.760772854001502</v>
+        <v>18.359330345228397</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="9"/>
-        <v>30.89434473575859</v>
+        <v>27.861720334803287</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="10"/>
-        <v>108.90893395225127</v>
+        <v>109.74333356427809</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="11"/>
-        <v>108.90893395225127</v>
+        <v>109.74333356427809</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="12"/>
-        <v>30.89434473575859</v>
+        <v>27.861720334803287</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="13"/>
-        <v>19.760772854001502</v>
+        <v>18.359330345228397</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="14"/>
-        <v>25.327558794880048</v>
+        <v>23.11052534001584</v>
       </c>
       <c r="AB5">
         <v>22.792100000000001</v>
@@ -20432,39 +20452,39 @@
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="7"/>
-        <v>24.565411408729222</v>
+        <v>30.680885596711807</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="8"/>
-        <v>22.505671474286657</v>
+        <v>18.269011418315554</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="9"/>
-        <v>25.831198074135095</v>
+        <v>30.117052544330104</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="10"/>
-        <v>55.021204965562973</v>
+        <v>110.41095666046003</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="11"/>
-        <v>65.977063789092384</v>
+        <v>110.41095666046003</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="12"/>
-        <v>25.831198074135095</v>
+        <v>30.117052544330104</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="13"/>
-        <v>22.505671474286657</v>
+        <v>18.269011418315554</v>
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="14"/>
-        <v>24.168434774210876</v>
+        <v>24.193031981322829</v>
       </c>
       <c r="AB6">
         <v>15.0762</v>
@@ -20516,35 +20536,35 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="7"/>
-        <v>31.854078448578456</v>
+        <v>25.864646486441941</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="8"/>
-        <v>23.570379825936332</v>
+        <v>23.520157241313434</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="9"/>
-        <v>30.649502373689785</v>
+        <v>26.715127698019575</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="10"/>
-        <v>103.71480772046159</v>
+        <v>103.66801115994332</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="11"/>
-        <v>103.71480772046159</v>
+        <v>103.66801115994332</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="12"/>
-        <v>30.649502373689785</v>
+        <v>26.715127698019575</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="13"/>
-        <v>23.570379825936332</v>
+        <v>23.520157241313434</v>
       </c>
       <c r="S7">
         <f t="shared" ca="1" si="14"/>
-        <v>27.109941099813057</v>
+        <v>25.117642469666507</v>
       </c>
       <c r="AB7">
         <v>11.031000000000001</v>
@@ -20592,39 +20612,39 @@
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="7"/>
-        <v>29.483074172304711</v>
+        <v>26.420748027777105</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="8"/>
-        <v>25.872094893808288</v>
+        <v>22.933491370605889</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="9"/>
-        <v>29.716359812581729</v>
+        <v>26.479623961825599</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="10"/>
-        <v>100.24218588728667</v>
+        <v>49.628544443785216</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="11"/>
-        <v>100.24218588728667</v>
+        <v>59.639932679079337</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="12"/>
-        <v>29.716359812581729</v>
+        <v>26.479623961825599</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="13"/>
-        <v>25.872094893808288</v>
+        <v>22.933491370605889</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="14"/>
-        <v>27.794227353195009</v>
+        <v>24.706557666215744</v>
       </c>
       <c r="AB8">
         <v>4.3186200000000001</v>
@@ -20672,39 +20692,39 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="7"/>
-        <v>20.111010443593891</v>
+        <v>28.207313473925989</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="8"/>
-        <v>21.543411204881259</v>
+        <v>17.338926267049509</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="9"/>
-        <v>22.032080317391458</v>
+        <v>27.861775571505913</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="10"/>
-        <v>47.266088756857634</v>
+        <v>94.948822284544448</v>
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="11"/>
-        <v>56.710794639210576</v>
+        <v>94.948822284544448</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="12"/>
-        <v>22.032080317391458</v>
+        <v>27.861775571505913</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="13"/>
-        <v>21.543411204881259</v>
+        <v>17.338926267049509</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="14"/>
-        <v>21.787745761136357</v>
+        <v>22.600350919277709</v>
       </c>
       <c r="AB9">
         <v>14.938499999999999</v>
@@ -20756,35 +20776,35 @@
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="7"/>
-        <v>29.161556675476817</v>
+        <v>25.281082222447218</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="8"/>
-        <v>16.474669220972544</v>
+        <v>16.784268409265042</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="9"/>
-        <v>27.735661403859748</v>
+        <v>25.797220892258956</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="10"/>
-        <v>89.220550422967122</v>
+        <v>89.069305904418229</v>
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="11"/>
-        <v>89.220550422967122</v>
+        <v>89.069305904418229</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="12"/>
-        <v>27.735661403859748</v>
+        <v>25.797220892258956</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="13"/>
-        <v>16.474669220972544</v>
+        <v>16.784268409265042</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="14"/>
-        <v>22.105165312416148</v>
+        <v>21.290744650762001</v>
       </c>
       <c r="AB10">
         <v>18.5778</v>
@@ -20832,39 +20852,39 @@
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="7"/>
-        <v>28.469012102716356</v>
+        <v>29.522605944349543</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="8"/>
-        <v>18.053235003050077</v>
+        <v>18.802611478000724</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="9"/>
-        <v>28.322341962945035</v>
+        <v>28.777528933931428</v>
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="10"/>
-        <v>43.59402671988731</v>
+        <v>87.235359291730873</v>
       </c>
       <c r="P11">
         <f t="shared" ca="1" si="11"/>
-        <v>52.283156131652021</v>
+        <v>87.235359291730873</v>
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="12"/>
-        <v>28.322341962945035</v>
+        <v>28.777528933931428</v>
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="13"/>
-        <v>18.053235003050077</v>
+        <v>18.802611478000724</v>
       </c>
       <c r="S11">
         <f t="shared" ca="1" si="14"/>
-        <v>23.187788482997554</v>
+        <v>23.790070205966074</v>
       </c>
       <c r="AB11">
         <v>11.5623</v>
@@ -20916,35 +20936,35 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="7"/>
-        <v>28.31464346775137</v>
+        <v>28.715961305034224</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="8"/>
-        <v>23.167308624116618</v>
+        <v>21.187910772477252</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="9"/>
-        <v>28.316183166790104</v>
+        <v>28.728274830813668</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="10"/>
-        <v>86.498022909629555</v>
+        <v>86.223633624579534</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="11"/>
-        <v>86.498022909629555</v>
+        <v>86.223633624579534</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="12"/>
-        <v>28.316183166790104</v>
+        <v>28.728274830813668</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="13"/>
-        <v>23.167308624116618</v>
+        <v>21.187910772477252</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="14"/>
-        <v>25.741745895453363</v>
+        <v>24.95809280164546</v>
       </c>
       <c r="AB12">
         <v>5.7392000000000003</v>
@@ -20996,35 +21016,35 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="7"/>
-        <v>27.39699278197422</v>
+        <v>27.853837849400037</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="8"/>
-        <v>24.655076988772485</v>
+        <v>20.509306205081604</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="9"/>
-        <v>27.5808308589374</v>
+        <v>28.028725245682764</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="10"/>
-        <v>84.616429143793454</v>
+        <v>85.459533230531918</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="11"/>
-        <v>84.616429143793454</v>
+        <v>85.459533230531918</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="12"/>
-        <v>27.5808308589374</v>
+        <v>28.028725245682764</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="13"/>
-        <v>24.655076988772485</v>
+        <v>20.509306205081604</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="14"/>
-        <v>26.117953923854941</v>
+        <v>24.269015725382182</v>
       </c>
       <c r="AB13">
         <v>14.312900000000001</v>
@@ -21076,35 +21096,35 @@
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="7"/>
-        <v>28.303404945635716</v>
+        <v>32.381059896928669</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="8"/>
-        <v>20.003146152757608</v>
+        <v>17.257214847628202</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="9"/>
-        <v>28.158890128296058</v>
+        <v>31.510592966679489</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="10"/>
-        <v>86.713639528818405</v>
+        <v>86.516150103653771</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="11"/>
-        <v>86.713639528818405</v>
+        <v>86.516150103653771</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="12"/>
-        <v>28.158890128296058</v>
+        <v>31.510592966679489</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="13"/>
-        <v>20.003146152757608</v>
+        <v>17.257214847628202</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="14"/>
-        <v>24.081018140526833</v>
+        <v>24.383903907153844</v>
       </c>
       <c r="AB14">
         <v>12.5059</v>
@@ -21152,39 +21172,39 @@
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="7"/>
-        <v>19.256433384672324</v>
+        <v>24.296040623717541</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="8"/>
-        <v>20.800721269909211</v>
+        <v>16.7947763832777</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="9"/>
-        <v>21.036924733397072</v>
+        <v>25.738951092309932</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="10"/>
-        <v>43.139874757613477</v>
+        <v>86.595876739797902</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="11"/>
-        <v>51.82900416937818</v>
+        <v>86.595876739797902</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="12"/>
-        <v>21.036924733397072</v>
+        <v>25.738951092309932</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="13"/>
-        <v>20.800721269909211</v>
+        <v>16.7947763832777</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="14"/>
-        <v>20.918823001653141</v>
+        <v>21.266863737793816</v>
       </c>
       <c r="AB15">
         <v>12.5343</v>
@@ -21232,39 +21252,39 @@
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="7"/>
-        <v>18.159488880780025</v>
+        <v>26.977637231097731</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="8"/>
-        <v>13.47555573541765</v>
+        <v>18.771918912222858</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="9"/>
-        <v>18.734976051303434</v>
+        <v>26.72990000334017</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="10"/>
-        <v>45.482341136398887</v>
+        <v>90.375259727370832</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="11"/>
-        <v>54.549258783457709</v>
+        <v>90.375259727370832</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="12"/>
-        <v>18.734976051303434</v>
+        <v>26.72990000334017</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="13"/>
-        <v>13.47555573541765</v>
+        <v>18.771918912222858</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="14"/>
-        <v>16.105265893360542</v>
+        <v>22.750909457781514</v>
       </c>
       <c r="AB16">
         <v>10.6838</v>
@@ -21316,35 +21336,35 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="7"/>
-        <v>29.412655772337718</v>
+        <v>29.732412542709906</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="8"/>
-        <v>17.68161513391777</v>
+        <v>16.647184988744243</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="9"/>
-        <v>27.277119828130864</v>
+        <v>29.131910034835961</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="10"/>
-        <v>91.298168066749824</v>
+        <v>90.519681934767718</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="11"/>
-        <v>91.298168066749824</v>
+        <v>90.519681934767718</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="12"/>
-        <v>27.277119828130864</v>
+        <v>29.131910034835961</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="13"/>
-        <v>17.68161513391777</v>
+        <v>16.647184988744243</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="14"/>
-        <v>22.479367481024319</v>
+        <v>22.889547511790102</v>
       </c>
       <c r="AB17">
         <v>10.097799999999999</v>
@@ -21392,39 +21412,39 @@
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="7"/>
-        <v>27.279294174286282</v>
+        <v>20.540628973777892</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="8"/>
-        <v>20.512459153581155</v>
+        <v>16.326498623696317</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="9"/>
-        <v>27.2788593050552</v>
+        <v>22.258885185989509</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="10"/>
-        <v>92.03016560939686</v>
+        <v>46.038648974559322</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="11"/>
-        <v>92.03016560939686</v>
+        <v>55.294460739265205</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="12"/>
-        <v>27.2788593050552</v>
+        <v>22.258885185989509</v>
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="13"/>
-        <v>20.512459153581155</v>
+        <v>16.326498623696317</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="14"/>
-        <v>23.895659229318177</v>
+        <v>19.292691904842911</v>
       </c>
       <c r="AB18">
         <v>9.4130400000000005</v>
@@ -21472,39 +21492,39 @@
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="7"/>
-        <v>29.342898766120825</v>
+        <v>25.03974672692323</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="8"/>
-        <v>23.726509238935968</v>
+        <v>14.790588376920999</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="9"/>
-        <v>28.930090873907702</v>
+        <v>24.483574418736488</v>
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="10"/>
-        <v>88.247577041710784</v>
+        <v>43.536833332364289</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="11"/>
-        <v>88.247577041710784</v>
+        <v>52.414856861776059</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="12"/>
-        <v>28.930090873907702</v>
+        <v>24.483574418736488</v>
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="13"/>
-        <v>23.726509238935968</v>
+        <v>14.790588376920999</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="14"/>
-        <v>26.328300056421835</v>
+        <v>19.637081397828744</v>
       </c>
       <c r="AB19">
         <v>8.5562000000000005</v>
@@ -21556,35 +21576,35 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="7"/>
-        <v>26.992356892473506</v>
+        <v>24.844414674816981</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="8"/>
-        <v>16.400273049616196</v>
+        <v>13.647592625090283</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="9"/>
-        <v>27.379903688760344</v>
+        <v>24.772246623600882</v>
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="10"/>
-        <v>94.746479047444765</v>
+        <v>95.297216806581318</v>
       </c>
       <c r="P20">
         <f t="shared" ca="1" si="11"/>
-        <v>94.746479047444765</v>
+        <v>95.297216806581318</v>
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="12"/>
-        <v>27.379903688760344</v>
+        <v>24.772246623600882</v>
       </c>
       <c r="R20">
         <f t="shared" ca="1" si="13"/>
-        <v>16.400273049616196</v>
+        <v>13.647592625090283</v>
       </c>
       <c r="S20">
         <f t="shared" ca="1" si="14"/>
-        <v>21.89008836918827</v>
+        <v>19.209919624345581</v>
       </c>
       <c r="AB20">
         <v>7.9345800000000004</v>
@@ -21632,39 +21652,39 @@
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="7"/>
-        <v>26.100808089940216</v>
+        <v>23.553005174107465</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="8"/>
-        <v>15.504728007808851</v>
+        <v>13.517109086458346</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="9"/>
-        <v>26.356627209704243</v>
+        <v>23.796853464006148</v>
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="10"/>
-        <v>91.334019052255726</v>
+        <v>45.297975968785927</v>
       </c>
       <c r="P21">
         <f t="shared" ca="1" si="11"/>
-        <v>91.334019052255726</v>
+        <v>54.36489361584475</v>
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="12"/>
-        <v>26.356627209704243</v>
+        <v>23.796853464006148</v>
       </c>
       <c r="R21">
         <f t="shared" ca="1" si="13"/>
-        <v>15.504728007808851</v>
+        <v>13.517109086458346</v>
       </c>
       <c r="S21">
         <f t="shared" ca="1" si="14"/>
-        <v>20.930677608756547</v>
+        <v>18.656981275232248</v>
       </c>
       <c r="AB21">
         <v>15.4214</v>
@@ -21712,39 +21732,39 @@
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="7"/>
-        <v>19.917959500389713</v>
+        <v>29.673248723678871</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="8"/>
-        <v>23.765302085637547</v>
+        <v>18.717095203175752</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="9"/>
-        <v>21.205693042252619</v>
+        <v>28.497969671744329</v>
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="10"/>
-        <v>47.410650245309242</v>
+        <v>94.12221143173619</v>
       </c>
       <c r="P22">
         <f t="shared" ca="1" si="11"/>
-        <v>56.855356127662183</v>
+        <v>94.12221143173619</v>
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="12"/>
-        <v>23.765302085637547</v>
+        <v>28.497969671744329</v>
       </c>
       <c r="R22">
         <f t="shared" ca="1" si="13"/>
-        <v>21.205693042252619</v>
+        <v>18.717095203175752</v>
       </c>
       <c r="S22">
         <f t="shared" ca="1" si="14"/>
-        <v>22.485497563945081</v>
+        <v>23.607532437460041</v>
       </c>
       <c r="AB22">
         <v>11.3246</v>
@@ -21796,35 +21816,35 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="7"/>
-        <v>18.31003928760958</v>
+        <v>21.606312128786666</v>
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="8"/>
-        <v>16.182544901829324</v>
+        <v>18.524278372461524</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="9"/>
-        <v>18.88917003853819</v>
+        <v>22.984643637378198</v>
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="10"/>
-        <v>46.005990561643841</v>
+        <v>45.875949719701822</v>
       </c>
       <c r="P23">
         <f t="shared" ca="1" si="11"/>
-        <v>55.261802326349724</v>
+        <v>55.131761484407704</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="12"/>
-        <v>18.88917003853819</v>
+        <v>22.984643637378198</v>
       </c>
       <c r="R23">
         <f t="shared" ca="1" si="13"/>
-        <v>16.182544901829324</v>
+        <v>18.524278372461524</v>
       </c>
       <c r="S23">
         <f t="shared" ca="1" si="14"/>
-        <v>17.535857470183757</v>
+        <v>20.754461004919861</v>
       </c>
       <c r="AB23">
         <v>7.1011600000000001</v>
@@ -21872,39 +21892,39 @@
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="7"/>
-        <v>23.056903697508051</v>
+        <v>27.483418742905489</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="8"/>
-        <v>14.487811051584201</v>
+        <v>20.71529030284762</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="9"/>
-        <v>22.223356965714082</v>
+        <v>26.583663721800033</v>
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="10"/>
-        <v>46.678731479532644</v>
+        <v>92.607262176590794</v>
       </c>
       <c r="P24">
         <f t="shared" ca="1" si="11"/>
-        <v>55.934543244238526</v>
+        <v>92.607262176590794</v>
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="12"/>
-        <v>22.223356965714082</v>
+        <v>26.583663721800033</v>
       </c>
       <c r="R24">
         <f t="shared" ca="1" si="13"/>
-        <v>14.487811051584201</v>
+        <v>20.71529030284762</v>
       </c>
       <c r="S24">
         <f t="shared" ca="1" si="14"/>
-        <v>18.355584008649142</v>
+        <v>23.649477012323828</v>
       </c>
       <c r="AB24">
         <v>11.790699999999999</v>
@@ -21952,39 +21972,39 @@
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="7"/>
-        <v>24.502408530079752</v>
+        <v>27.844125206326009</v>
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="8"/>
-        <v>22.578928657385088</v>
+        <v>19.474879279340399</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="9"/>
-        <v>24.046598217206618</v>
+        <v>27.592032909420816</v>
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="10"/>
-        <v>47.735273510810565</v>
+        <v>94.207115903211161</v>
       </c>
       <c r="P25">
         <f t="shared" ca="1" si="11"/>
-        <v>57.179979393163507</v>
+        <v>94.207115903211161</v>
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="12"/>
-        <v>24.046598217206618</v>
+        <v>27.592032909420816</v>
       </c>
       <c r="R25">
         <f t="shared" ca="1" si="13"/>
-        <v>22.578928657385088</v>
+        <v>19.474879279340399</v>
       </c>
       <c r="S25">
         <f t="shared" ca="1" si="14"/>
-        <v>23.312763437295853</v>
+        <v>23.533456094380607</v>
       </c>
       <c r="AB25">
         <v>7.1720600000000001</v>
@@ -22036,35 +22056,35 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="7"/>
-        <v>19.504523674748533</v>
+        <v>32.588939842286827</v>
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="8"/>
-        <v>18.178854522817993</v>
+        <v>12.774441542397964</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="9"/>
-        <v>20.412938583240152</v>
+        <v>31.589558455713629</v>
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="10"/>
-        <v>92.793250186515706</v>
+        <v>91.935005122360849</v>
       </c>
       <c r="P26">
         <f t="shared" ca="1" si="11"/>
-        <v>92.793250186515706</v>
+        <v>91.935005122360849</v>
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="12"/>
-        <v>20.412938583240152</v>
+        <v>31.589558455713629</v>
       </c>
       <c r="R26">
         <f t="shared" ca="1" si="13"/>
-        <v>18.178854522817993</v>
+        <v>12.774441542397964</v>
       </c>
       <c r="S26">
         <f t="shared" ca="1" si="14"/>
-        <v>19.295896553029074</v>
+        <v>22.181999999055797</v>
       </c>
       <c r="AB26">
         <v>11.055199999999999</v>
@@ -22116,35 +22136,35 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="7"/>
-        <v>23.440086373041304</v>
+        <v>20.04140286628018</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="8"/>
-        <v>21.310738945384273</v>
+        <v>16.201720618556866</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="9"/>
-        <v>22.834656815081075</v>
+        <v>22.351033984166872</v>
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="10"/>
-        <v>44.139522966515806</v>
+        <v>44.192833903096769</v>
       </c>
       <c r="P27">
         <f t="shared" ca="1" si="11"/>
-        <v>53.017546495927576</v>
+        <v>53.070857432508532</v>
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="12"/>
-        <v>22.834656815081075</v>
+        <v>22.351033984166872</v>
       </c>
       <c r="R27">
         <f t="shared" ca="1" si="13"/>
-        <v>21.310738945384273</v>
+        <v>16.201720618556866</v>
       </c>
       <c r="S27">
         <f t="shared" ca="1" si="14"/>
-        <v>22.072697880232674</v>
+        <v>19.276377301361869</v>
       </c>
       <c r="AB27">
         <v>5.6329700000000003</v>
@@ -22192,39 +22212,39 @@
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="7"/>
-        <v>25.48952847818725</v>
+        <v>23.455323184482378</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="8"/>
-        <v>17.464349368681553</v>
+        <v>12.634186534345524</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="9"/>
-        <v>24.958554145566019</v>
+        <v>23.234465344419277</v>
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="10"/>
-        <v>90.370756735941782</v>
+        <v>44.911533440695862</v>
       </c>
       <c r="P28">
         <f t="shared" ca="1" si="11"/>
-        <v>90.370756735941782</v>
+        <v>53.978451087754685</v>
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="12"/>
-        <v>24.958554145566019</v>
+        <v>23.234465344419277</v>
       </c>
       <c r="R28">
         <f t="shared" ca="1" si="13"/>
-        <v>17.464349368681553</v>
+        <v>12.634186534345524</v>
       </c>
       <c r="S28">
         <f t="shared" ca="1" si="14"/>
-        <v>21.211451757123786</v>
+        <v>17.934325939382401</v>
       </c>
       <c r="AB28">
         <v>4.3788200000000002</v>
@@ -22276,35 +22296,35 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="7"/>
-        <v>23.991350846152329</v>
+        <v>24.77785586168158</v>
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="8"/>
-        <v>17.147833977484773</v>
+        <v>15.112027072439044</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="9"/>
-        <v>24.184791506035069</v>
+        <v>24.469177758229122</v>
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="10"/>
-        <v>90.577495052639293</v>
+        <v>91.076865674527227</v>
       </c>
       <c r="P29">
         <f t="shared" ca="1" si="11"/>
-        <v>90.577495052639293</v>
+        <v>91.076865674527227</v>
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="12"/>
-        <v>24.184791506035069</v>
+        <v>24.469177758229122</v>
       </c>
       <c r="R29">
         <f t="shared" ca="1" si="13"/>
-        <v>17.147833977484773</v>
+        <v>15.112027072439044</v>
       </c>
       <c r="S29">
         <f t="shared" ca="1" si="14"/>
-        <v>20.666312741759921</v>
+        <v>19.790602415334085</v>
       </c>
       <c r="AB29">
         <v>7.12798</v>
@@ -22356,35 +22376,35 @@
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="7"/>
-        <v>25.538625029335126</v>
+        <v>26.619187840122468</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="8"/>
-        <v>10.196004409124351</v>
+        <v>10.996984679591822</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="9"/>
-        <v>25.267858324675117</v>
+        <v>26.189185823743802</v>
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="10"/>
-        <v>86.355441310054687</v>
+        <v>86.460776735612825</v>
       </c>
       <c r="P30">
         <f t="shared" ca="1" si="11"/>
-        <v>86.355441310054687</v>
+        <v>86.460776735612825</v>
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="12"/>
-        <v>25.267858324675117</v>
+        <v>26.189185823743802</v>
       </c>
       <c r="R30">
         <f t="shared" ca="1" si="13"/>
-        <v>10.196004409124351</v>
+        <v>10.996984679591822</v>
       </c>
       <c r="S30">
         <f t="shared" ca="1" si="14"/>
-        <v>17.731931366899733</v>
+        <v>18.593085251667812</v>
       </c>
       <c r="AB30">
         <v>3.10764</v>
@@ -22436,35 +22456,35 @@
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="7"/>
-        <v>25.553758673485518</v>
+        <v>29.153239606802373</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="8"/>
-        <v>16.597882564959697</v>
+        <v>14.728821539318091</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="9"/>
-        <v>25.496578603723439</v>
+        <v>28.560428850190661</v>
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="10"/>
-        <v>88.70356188739342</v>
+        <v>88.757132702114163</v>
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="11"/>
-        <v>88.70356188739342</v>
+        <v>88.757132702114163</v>
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="12"/>
-        <v>25.496578603723439</v>
+        <v>28.560428850190661</v>
       </c>
       <c r="R31">
         <f t="shared" ca="1" si="13"/>
-        <v>16.597882564959697</v>
+        <v>14.728821539318091</v>
       </c>
       <c r="S31">
         <f t="shared" ca="1" si="14"/>
-        <v>21.04723058434157</v>
+        <v>21.644625194754376</v>
       </c>
       <c r="AB31">
         <v>11.0318</v>
@@ -22516,35 +22536,35 @@
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="7"/>
-        <v>26.819724100224622</v>
+        <v>20.329509874936363</v>
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="8"/>
-        <v>13.695562075582753</v>
+        <v>8.7474648244060909</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="9"/>
-        <v>26.555095000924386</v>
+        <v>21.975693669987223</v>
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="10"/>
-        <v>88.465179612272934</v>
+        <v>89.294092413167022</v>
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="11"/>
-        <v>88.465179612272934</v>
+        <v>89.294092413167022</v>
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="12"/>
-        <v>26.555095000924386</v>
+        <v>21.975693669987223</v>
       </c>
       <c r="R32">
         <f t="shared" ca="1" si="13"/>
-        <v>13.695562075582753</v>
+        <v>8.7474648244060909</v>
       </c>
       <c r="S32">
         <f t="shared" ca="1" si="14"/>
-        <v>20.125328538253569</v>
+        <v>15.361579247196657</v>
       </c>
       <c r="AB32">
         <v>1.65354</v>
@@ -22611,35 +22631,35 @@
       </c>
       <c r="K34">
         <f ca="1">COUNTIF(K3:K33,"&gt;0")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L34" s="4">
         <f ca="1">AVERAGE(L3:L32)</f>
-        <v>25.746367111440957</v>
+        <v>26.732655762878444</v>
       </c>
       <c r="M34" s="4">
         <f ca="1">AVERAGE(M3:M32)</f>
-        <v>19.263575117776828</v>
+        <v>17.381533859832054</v>
       </c>
       <c r="N34" s="4">
         <f ca="1">AVERAGE(N3:N32)</f>
-        <v>25.809467325536833</v>
+        <v>26.819264162767347</v>
       </c>
       <c r="O34" s="4">
         <f ca="1">AVERAGE(O3:O32)</f>
-        <v>78.011270072068683</v>
+        <v>81.023136083213572</v>
       </c>
       <c r="Q34" s="8">
         <f ca="1">AVERAGE(Q3:Q32)</f>
-        <v>25.894787626982996</v>
+        <v>26.819264162767347</v>
       </c>
       <c r="R34" s="8">
         <f ca="1">AVERAGE(R3:R32)</f>
-        <v>19.178254816330661</v>
+        <v>17.381533859832054</v>
       </c>
       <c r="S34">
         <f ca="1">AVERAGE(S3:S32)</f>
-        <v>22.536521221656827</v>
+        <v>22.100399011299704</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
@@ -22666,27 +22686,27 @@
       </c>
       <c r="L35">
         <f ca="1">_xlfn.STDEV.P(L3:L32)</f>
-        <v>4.0889566615175594</v>
+        <v>3.4092748808747508</v>
       </c>
       <c r="M35">
         <f t="shared" ref="M35:N35" ca="1" si="18">_xlfn.STDEV.P(M3:M32)</f>
-        <v>3.7406875025060944</v>
+        <v>3.704663997251493</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="18"/>
-        <v>3.624478628251885</v>
+        <v>2.797867479856524</v>
       </c>
       <c r="O35">
         <f t="shared" ref="O35" ca="1" si="19">_xlfn.STDEV.P(O3:O32)</f>
-        <v>23.176312531162473</v>
+        <v>21.807606410371513</v>
       </c>
       <c r="Q35">
         <f ca="1">_xlfn.STDEV.P(Q3:Q32)</f>
-        <v>3.5443421912538073</v>
+        <v>2.797867479856524</v>
       </c>
       <c r="R35">
         <f ca="1">_xlfn.STDEV.P(R3:R32)</f>
-        <v>3.6654703175554459</v>
+        <v>3.704663997251493</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
@@ -35066,15 +35086,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D371"/>
+  <dimension ref="A1:I371"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -35082,7 +35102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -35090,8 +35110,16 @@
         <f>RADIANS(23.4)</f>
         <v>0.40840704496667307</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>30*12</f>
+        <v>360</v>
+      </c>
+      <c r="I2">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -35099,17 +35127,40 @@
         <f>RADIANS(36.7833)</f>
         <v>0.64198969474883016</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f>365/2</f>
+        <v>182.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>141</v>
       </c>
       <c r="B4">
-        <f>1 - TAN(B3) * TAN(B2 * COS(PI()*B1/182.625))</f>
-        <v>0.68413488963337166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5">
+        <f>MAX(C$7:C$371)</f>
+        <v>15.882307754758394</v>
+      </c>
+      <c r="H5">
+        <f>MAX(D$7:D$371)</f>
+        <v>15.882358041015024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -35122,8 +35173,19 @@
       <c r="D6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6">
+        <f>MIN(C$7:C$371)</f>
+        <v>8.1176419589849758</v>
+      </c>
+      <c r="H6">
+        <f>MIN(D$7:D$371)</f>
+        <v>8.1176922452416065</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -35139,8 +35201,19 @@
         <f>24-C7</f>
         <v>15.881754632282519</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7">
+        <f>AVERAGE(C$7:C$371)</f>
+        <v>12.002659149342634</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(D$7:D$371)</f>
+        <v>11.997340850657363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -35157,7 +35230,7 @@
         <v>15.879824110533656</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -35174,7 +35247,7 @@
         <v>15.876607881246933</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -35191,7 +35264,7 @@
         <v>15.87210790208549</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -35208,7 +35281,7 @@
         <v>15.866326908231606</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -35225,7 +35298,7 @@
         <v>15.859268406867852</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
@@ -35242,7 +35315,7 @@
         <v>15.850936670120248</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -35259,7 +35332,7 @@
         <v>15.841336726492155</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9</v>
       </c>
@@ -35276,7 +35349,7 @@
         <v>15.830474350823685</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Working on seed production and flowering, issue #2
</commit_message>
<xml_diff>
--- a/Design docs/sunlightstats.xlsx
+++ b/Design docs/sunlightstats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="25875" windowHeight="11370" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="25875" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="raws" sheetId="1" r:id="rId1"/>
@@ -833,94 +833,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>32.368701656654501</c:v>
+                  <c:v>29.316922501816855</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.391405596902064</c:v>
+                  <c:v>30.97904619475829</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.861720334803287</c:v>
+                  <c:v>30.031892208565473</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.117052544330104</c:v>
+                  <c:v>26.809197646081287</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.715127698019575</c:v>
+                  <c:v>28.690601511623402</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.479623961825599</c:v>
+                  <c:v>29.65888301636889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.861775571505913</c:v>
+                  <c:v>21.514219844190961</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.797220892258956</c:v>
+                  <c:v>22.987219073310218</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.777528933931428</c:v>
+                  <c:v>28.674304891611857</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28.728274830813668</c:v>
+                  <c:v>30.145075335310359</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.028725245682764</c:v>
+                  <c:v>27.631571506581061</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31.510592966679489</c:v>
+                  <c:v>19.320872182133268</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25.738951092309932</c:v>
+                  <c:v>29.087034502204762</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.72990000334017</c:v>
+                  <c:v>26.211403470825342</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.131910034835961</c:v>
+                  <c:v>24.061530523727789</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.258885185989509</c:v>
+                  <c:v>25.310105857542343</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.483574418736488</c:v>
+                  <c:v>31.965920477434828</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.772246623600882</c:v>
+                  <c:v>26.00286517636761</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23.796853464006148</c:v>
+                  <c:v>25.980364383230306</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28.497969671744329</c:v>
+                  <c:v>23.198667274345887</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22.984643637378198</c:v>
+                  <c:v>27.022802204279763</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26.583663721800033</c:v>
+                  <c:v>23.970195388935682</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27.592032909420816</c:v>
+                  <c:v>24.320081386090607</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31.589558455713629</c:v>
+                  <c:v>26.137939390529226</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.351033984166872</c:v>
+                  <c:v>23.337836929808596</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.234465344419277</c:v>
+                  <c:v>25.914493389464141</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>24.469177758229122</c:v>
+                  <c:v>27.684971010600016</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>26.189185823743802</c:v>
+                  <c:v>23.763507841353007</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.560428850190661</c:v>
+                  <c:v>26.39028954912866</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>21.975693669987223</c:v>
+                  <c:v>26.541697152517855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,94 +956,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>25.215260395062391</c:v>
+                  <c:v>16.859712771399856</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.145668079642252</c:v>
+                  <c:v>18.814460679903792</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.359330345228397</c:v>
+                  <c:v>17.594292517835736</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.269011418315554</c:v>
+                  <c:v>19.195241280878182</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.520157241313434</c:v>
+                  <c:v>20.752612739860062</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.933491370605889</c:v>
+                  <c:v>21.627524019215297</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.338926267049509</c:v>
+                  <c:v>17.073494649460251</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.784268409265042</c:v>
+                  <c:v>18.339391175479683</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.802611478000724</c:v>
+                  <c:v>20.392869106376001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.187910772477252</c:v>
+                  <c:v>18.780270113741288</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.509306205081604</c:v>
+                  <c:v>19.187155010159472</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.257214847628202</c:v>
+                  <c:v>14.522460471368635</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.7947763832777</c:v>
+                  <c:v>16.553644441058694</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.771918912222858</c:v>
+                  <c:v>15.240517004233212</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.647184988744243</c:v>
+                  <c:v>12.603060224198551</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.326498623696317</c:v>
+                  <c:v>15.08445549770784</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.790588376920999</c:v>
+                  <c:v>10.274496415490045</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.647592625090283</c:v>
+                  <c:v>14.245589611344045</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.517109086458346</c:v>
+                  <c:v>19.167117909755781</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18.717095203175752</c:v>
+                  <c:v>19.338634690717473</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.524278372461524</c:v>
+                  <c:v>16.552374345472636</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20.71529030284762</c:v>
+                  <c:v>15.096427487120485</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19.474879279340399</c:v>
+                  <c:v>17.083125420105304</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.774441542397964</c:v>
+                  <c:v>15.291077759443521</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16.201720618556866</c:v>
+                  <c:v>12.371485891951234</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.634186534345524</c:v>
+                  <c:v>17.464792035564781</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15.112027072439044</c:v>
+                  <c:v>11.973883633289953</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.996984679591822</c:v>
+                  <c:v>20.625141346192805</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14.728821539318091</c:v>
+                  <c:v>13.646789583005873</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.7474648244060909</c:v>
+                  <c:v>14.753841207099613</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,11 +1060,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184179200"/>
-        <c:axId val="166497088"/>
+        <c:axId val="174414336"/>
+        <c:axId val="146639680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184179200"/>
+        <c:axId val="174414336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1073,7 +1073,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166497088"/>
+        <c:crossAx val="146639680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1081,7 +1081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166497088"/>
+        <c:axId val="146639680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1111,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184179200"/>
+        <c:crossAx val="174414336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1398,11 +1398,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184463360"/>
-        <c:axId val="166499392"/>
+        <c:axId val="174698496"/>
+        <c:axId val="146641984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184463360"/>
+        <c:axId val="174698496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166499392"/>
+        <c:crossAx val="146641984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166499392"/>
+        <c:axId val="146641984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184463360"/>
+        <c:crossAx val="174698496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1484,94 +1484,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>111.84024915523568</c:v>
+                  <c:v>111.3098112466526</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.847910366204488</c:v>
+                  <c:v>107.34284984908234</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109.74333356427809</c:v>
+                  <c:v>109.52907121528061</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.41095666046003</c:v>
+                  <c:v>109.36398978595108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.66801115994332</c:v>
+                  <c:v>103.46519993019399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.628544443785216</c:v>
+                  <c:v>99.696449699729357</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94.948822284544448</c:v>
+                  <c:v>47.275334596998661</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.069305904418229</c:v>
+                  <c:v>44.114678007454344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.235359291730873</c:v>
+                  <c:v>87.093775055812671</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86.223633624579534</c:v>
+                  <c:v>87.491803613286578</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>85.459533230531918</c:v>
+                  <c:v>84.72731391074278</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>86.516150103653771</c:v>
+                  <c:v>42.986723412771944</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>86.595876739797902</c:v>
+                  <c:v>87.176621471075379</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90.375259727370832</c:v>
+                  <c:v>90.435116104374529</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90.519681934767718</c:v>
+                  <c:v>90.889902718555419</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46.038648974559322</c:v>
+                  <c:v>92.396401778633063</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43.536833332364289</c:v>
+                  <c:v>88.92878956524028</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>95.297216806581318</c:v>
+                  <c:v>94.344816931383491</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>45.297975968785927</c:v>
+                  <c:v>90.503750467150283</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>94.12221143173619</c:v>
+                  <c:v>94.748922842168326</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>45.875949719701822</c:v>
+                  <c:v>92.741841782295452</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>92.607262176590794</c:v>
+                  <c:v>92.471995593560422</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>94.207115903211161</c:v>
+                  <c:v>47.129289132197414</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>91.935005122360849</c:v>
+                  <c:v>46.083081819018801</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44.192833903096769</c:v>
+                  <c:v>88.475238227270992</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44.911533440695862</c:v>
+                  <c:v>90.459632769749092</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>91.076865674527227</c:v>
+                  <c:v>91.124527115754532</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>86.460776735612825</c:v>
+                  <c:v>87.322885627599717</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>88.757132702114163</c:v>
+                  <c:v>88.136555721268451</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>89.294092413167022</c:v>
+                  <c:v>89.274029588135974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1591,94 +1591,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>111.84024915523568</c:v>
+                  <c:v>111.3098112466526</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.614875072086846</c:v>
+                  <c:v>107.34284984908234</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109.74333356427809</c:v>
+                  <c:v>109.52907121528061</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.41095666046003</c:v>
+                  <c:v>109.36398978595108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.66801115994332</c:v>
+                  <c:v>103.46519993019399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59.639932679079337</c:v>
+                  <c:v>99.696449699729357</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94.948822284544448</c:v>
+                  <c:v>56.720040479351603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.069305904418229</c:v>
+                  <c:v>52.992701536866107</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.235359291730873</c:v>
+                  <c:v>87.093775055812671</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86.223633624579534</c:v>
+                  <c:v>87.491803613286578</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>85.459533230531918</c:v>
+                  <c:v>84.72731391074278</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>86.516150103653771</c:v>
+                  <c:v>51.675852824536648</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>86.595876739797902</c:v>
+                  <c:v>87.176621471075379</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90.375259727370832</c:v>
+                  <c:v>90.435116104374529</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90.519681934767718</c:v>
+                  <c:v>90.889902718555419</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>55.294460739265205</c:v>
+                  <c:v>92.396401778633063</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>52.414856861776059</c:v>
+                  <c:v>88.92878956524028</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>95.297216806581318</c:v>
+                  <c:v>94.344816931383491</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>54.36489361584475</c:v>
+                  <c:v>90.503750467150283</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>94.12221143173619</c:v>
+                  <c:v>94.748922842168326</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>55.131761484407704</c:v>
+                  <c:v>92.741841782295452</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>92.607262176590794</c:v>
+                  <c:v>92.471995593560422</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>94.207115903211161</c:v>
+                  <c:v>56.573995014550356</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>91.935005122360849</c:v>
+                  <c:v>55.338893583724683</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53.070857432508532</c:v>
+                  <c:v>88.475238227270992</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>53.978451087754685</c:v>
+                  <c:v>90.459632769749092</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>91.076865674527227</c:v>
+                  <c:v>91.124527115754532</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>86.460776735612825</c:v>
+                  <c:v>87.322885627599717</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>88.757132702114163</c:v>
+                  <c:v>88.136555721268451</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>89.294092413167022</c:v>
+                  <c:v>89.274029588135974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1695,11 +1695,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184464896"/>
-        <c:axId val="166501120"/>
+        <c:axId val="174700032"/>
+        <c:axId val="146643712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184464896"/>
+        <c:axId val="174700032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166501120"/>
+        <c:crossAx val="146643712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +1716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166501120"/>
+        <c:axId val="146643712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184464896"/>
+        <c:crossAx val="174700032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2895,11 +2895,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="184465408"/>
-        <c:axId val="191242816"/>
+        <c:axId val="174700544"/>
+        <c:axId val="194060864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="184465408"/>
+        <c:axId val="174700544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2908,7 +2908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191242816"/>
+        <c:crossAx val="194060864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2916,7 +2916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191242816"/>
+        <c:axId val="194060864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2927,7 +2927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184465408"/>
+        <c:crossAx val="174700544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4071,8 +4071,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="184466944"/>
-        <c:axId val="191244544"/>
+        <c:axId val="174702080"/>
+        <c:axId val="194062592"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6279,11 +6279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="191119872"/>
-        <c:axId val="191245120"/>
+        <c:axId val="182870528"/>
+        <c:axId val="194063168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184466944"/>
+        <c:axId val="174702080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6292,7 +6292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191244544"/>
+        <c:crossAx val="194062592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6300,7 +6300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191244544"/>
+        <c:axId val="194062592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6311,12 +6311,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184466944"/>
+        <c:crossAx val="174702080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191245120"/>
+        <c:axId val="194063168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6326,12 +6326,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191119872"/>
+        <c:crossAx val="182870528"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="191119872"/>
+        <c:axId val="182870528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6340,7 +6340,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191245120"/>
+        <c:crossAx val="194063168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7520,8 +7520,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="191121920"/>
-        <c:axId val="191248000"/>
+        <c:axId val="182872576"/>
+        <c:axId val="194066048"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9788,11 +9788,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="191120896"/>
-        <c:axId val="191247424"/>
+        <c:axId val="182871552"/>
+        <c:axId val="194065472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="191120896"/>
+        <c:axId val="182871552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9801,7 +9801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191247424"/>
+        <c:crossAx val="194065472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9809,7 +9809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191247424"/>
+        <c:axId val="194065472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9820,12 +9820,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191120896"/>
+        <c:crossAx val="182871552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191248000"/>
+        <c:axId val="194066048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9835,12 +9835,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191121920"/>
+        <c:crossAx val="182872576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="191121920"/>
+        <c:axId val="182872576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9849,7 +9849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191248000"/>
+        <c:crossAx val="194066048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11035,11 +11035,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="191122432"/>
-        <c:axId val="191594496"/>
+        <c:axId val="182873088"/>
+        <c:axId val="194412544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="191122432"/>
+        <c:axId val="182873088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11048,7 +11048,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191594496"/>
+        <c:crossAx val="194412544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11056,7 +11056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191594496"/>
+        <c:axId val="194412544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11067,7 +11067,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191122432"/>
+        <c:crossAx val="182873088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13343,8 +13343,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191596224"/>
-        <c:axId val="191596800"/>
+        <c:axId val="194414272"/>
+        <c:axId val="194414848"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -15584,11 +15584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191597952"/>
-        <c:axId val="191597376"/>
+        <c:axId val="194416000"/>
+        <c:axId val="194415424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="191596224"/>
+        <c:axId val="194414272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15598,12 +15598,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191596800"/>
+        <c:crossAx val="194414848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191596800"/>
+        <c:axId val="194414848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15614,12 +15614,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191596224"/>
+        <c:crossAx val="194414272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191597376"/>
+        <c:axId val="194415424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15629,12 +15629,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191597952"/>
+        <c:crossAx val="194416000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191597952"/>
+        <c:axId val="194416000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15644,7 +15644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191597376"/>
+        <c:crossAx val="194415424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16212,7 +16212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -20216,35 +20216,35 @@
       </c>
       <c r="L3">
         <f ca="1">_xlfn.NORM.INV(RAND(), IF(K3=1,E3,F3), $B$35)</f>
-        <v>32.368701656654501</v>
+        <v>29.316922501816855</v>
       </c>
       <c r="M3">
         <f ca="1">_xlfn.NORM.INV(RAND(), G3, $C$35/3)</f>
-        <v>25.215260395062391</v>
+        <v>16.859712771399856</v>
       </c>
       <c r="N3">
         <f ca="1">L3</f>
-        <v>32.368701656654501</v>
+        <v>29.316922501816855</v>
       </c>
       <c r="O3">
         <f ca="1">_xlfn.NORM.INV(RAND(), IF(K3=1,J3,I3), $D$35)</f>
-        <v>111.84024915523568</v>
+        <v>111.3098112466526</v>
       </c>
       <c r="P3">
         <f ca="1">IF(K3=1, O3 + 0.1 * I3, O3)</f>
-        <v>111.84024915523568</v>
+        <v>111.3098112466526</v>
       </c>
       <c r="Q3">
         <f ca="1">IF(N3 &lt; M3, M3, N3)</f>
-        <v>32.368701656654501</v>
+        <v>29.316922501816855</v>
       </c>
       <c r="R3">
         <f ca="1">IF(N3 &lt; M3, N3, M3)</f>
-        <v>25.215260395062391</v>
+        <v>16.859712771399856</v>
       </c>
       <c r="S3">
         <f ca="1">AVERAGE(Q3,R3)</f>
-        <v>28.791981025858448</v>
+        <v>23.088317636608355</v>
       </c>
       <c r="AB3">
         <v>12.581799999999999</v>
@@ -20292,39 +20292,39 @@
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L32" ca="1" si="7">_xlfn.NORM.INV(RAND(), IF(K4=1,E4,F4), $B$35)</f>
-        <v>28.647081581963953</v>
+        <v>31.394577117993649</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M32" ca="1" si="8">_xlfn.NORM.INV(RAND(), G4, $C$35/3)</f>
-        <v>22.145668079642252</v>
+        <v>18.814460679903792</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N32" ca="1" si="9">N3 * $N$1 + (1-$N$1) * L4</f>
-        <v>29.391405596902064</v>
+        <v>30.97904619475829</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O32" ca="1" si="10">_xlfn.NORM.INV(RAND(), IF(K4=1,J4,I4), $D$35)</f>
-        <v>54.847910366204488</v>
+        <v>107.34284984908234</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P32" ca="1" si="11">IF(K4=1, O4 + 0.1 * I4, O4)</f>
-        <v>65.614875072086846</v>
+        <v>107.34284984908234</v>
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q32" ca="1" si="12">IF(N4 &lt; M4, M4, N4)</f>
-        <v>29.391405596902064</v>
+        <v>30.97904619475829</v>
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R32" ca="1" si="13">IF(N4 &lt; M4, N4, M4)</f>
-        <v>22.145668079642252</v>
+        <v>18.814460679903792</v>
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S32" ca="1" si="14">AVERAGE(Q4,R4)</f>
-        <v>25.768536838272158</v>
+        <v>24.896753437331043</v>
       </c>
       <c r="AB4">
         <v>8.5861499999999999</v>
@@ -20376,35 +20376,35 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="7"/>
-        <v>27.479299019278589</v>
+        <v>29.795103712017269</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="8"/>
-        <v>18.359330345228397</v>
+        <v>17.594292517835736</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="9"/>
-        <v>27.861720334803287</v>
+        <v>30.031892208565473</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="10"/>
-        <v>109.74333356427809</v>
+        <v>109.52907121528061</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="11"/>
-        <v>109.74333356427809</v>
+        <v>109.52907121528061</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="12"/>
-        <v>27.861720334803287</v>
+        <v>30.031892208565473</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="13"/>
-        <v>18.359330345228397</v>
+        <v>17.594292517835736</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="14"/>
-        <v>23.11052534001584</v>
+        <v>23.813092363200603</v>
       </c>
       <c r="AB5">
         <v>22.792100000000001</v>
@@ -20456,35 +20456,35 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="7"/>
-        <v>30.680885596711807</v>
+        <v>26.003524005460239</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="8"/>
-        <v>18.269011418315554</v>
+        <v>19.195241280878182</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="9"/>
-        <v>30.117052544330104</v>
+        <v>26.809197646081287</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="10"/>
-        <v>110.41095666046003</v>
+        <v>109.36398978595108</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="11"/>
-        <v>110.41095666046003</v>
+        <v>109.36398978595108</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="12"/>
-        <v>30.117052544330104</v>
+        <v>26.809197646081287</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="13"/>
-        <v>18.269011418315554</v>
+        <v>19.195241280878182</v>
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="14"/>
-        <v>24.193031981322829</v>
+        <v>23.002219463479733</v>
       </c>
       <c r="AB6">
         <v>15.0762</v>
@@ -20536,35 +20536,35 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="7"/>
-        <v>25.864646486441941</v>
+        <v>29.16095247800893</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="8"/>
-        <v>23.520157241313434</v>
+        <v>20.752612739860062</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="9"/>
-        <v>26.715127698019575</v>
+        <v>28.690601511623402</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="10"/>
-        <v>103.66801115994332</v>
+        <v>103.46519993019399</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="11"/>
-        <v>103.66801115994332</v>
+        <v>103.46519993019399</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="12"/>
-        <v>26.715127698019575</v>
+        <v>28.690601511623402</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="13"/>
-        <v>23.520157241313434</v>
+        <v>20.752612739860062</v>
       </c>
       <c r="S7">
         <f t="shared" ca="1" si="14"/>
-        <v>25.117642469666507</v>
+        <v>24.721607125741734</v>
       </c>
       <c r="AB7">
         <v>11.031000000000001</v>
@@ -20612,39 +20612,39 @@
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="7"/>
-        <v>26.420748027777105</v>
+        <v>29.900953392555259</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="8"/>
-        <v>22.933491370605889</v>
+        <v>21.627524019215297</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="9"/>
-        <v>26.479623961825599</v>
+        <v>29.65888301636889</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="10"/>
-        <v>49.628544443785216</v>
+        <v>99.696449699729357</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="11"/>
-        <v>59.639932679079337</v>
+        <v>99.696449699729357</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="12"/>
-        <v>26.479623961825599</v>
+        <v>29.65888301636889</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="13"/>
-        <v>22.933491370605889</v>
+        <v>21.627524019215297</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="14"/>
-        <v>24.706557666215744</v>
+        <v>25.643203517792095</v>
       </c>
       <c r="AB8">
         <v>4.3186200000000001</v>
@@ -20692,39 +20692,39 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="7"/>
-        <v>28.207313473925989</v>
+        <v>19.478054051146476</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="8"/>
-        <v>17.338926267049509</v>
+        <v>17.073494649460251</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="9"/>
-        <v>27.861775571505913</v>
+        <v>21.514219844190961</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="10"/>
-        <v>94.948822284544448</v>
+        <v>47.275334596998661</v>
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="11"/>
-        <v>94.948822284544448</v>
+        <v>56.720040479351603</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="12"/>
-        <v>27.861775571505913</v>
+        <v>21.514219844190961</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="13"/>
-        <v>17.338926267049509</v>
+        <v>17.073494649460251</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="14"/>
-        <v>22.600350919277709</v>
+        <v>19.293857246825606</v>
       </c>
       <c r="AB9">
         <v>14.938499999999999</v>
@@ -20772,39 +20772,39 @@
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="7"/>
-        <v>25.281082222447218</v>
+        <v>23.355468880590031</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="8"/>
-        <v>16.784268409265042</v>
+        <v>18.339391175479683</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="9"/>
-        <v>25.797220892258956</v>
+        <v>22.987219073310218</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="10"/>
-        <v>89.069305904418229</v>
+        <v>44.114678007454344</v>
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="11"/>
-        <v>89.069305904418229</v>
+        <v>52.992701536866107</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="12"/>
-        <v>25.797220892258956</v>
+        <v>22.987219073310218</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="13"/>
-        <v>16.784268409265042</v>
+        <v>18.339391175479683</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="14"/>
-        <v>21.290744650762001</v>
+        <v>20.663305124394952</v>
       </c>
       <c r="AB10">
         <v>18.5778</v>
@@ -20856,35 +20856,35 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="7"/>
-        <v>29.522605944349543</v>
+        <v>30.096076346187267</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="8"/>
-        <v>18.802611478000724</v>
+        <v>20.392869106376001</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="9"/>
-        <v>28.777528933931428</v>
+        <v>28.674304891611857</v>
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="10"/>
-        <v>87.235359291730873</v>
+        <v>87.093775055812671</v>
       </c>
       <c r="P11">
         <f t="shared" ca="1" si="11"/>
-        <v>87.235359291730873</v>
+        <v>87.093775055812671</v>
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="12"/>
-        <v>28.777528933931428</v>
+        <v>28.674304891611857</v>
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="13"/>
-        <v>18.802611478000724</v>
+        <v>20.392869106376001</v>
       </c>
       <c r="S11">
         <f t="shared" ca="1" si="14"/>
-        <v>23.790070205966074</v>
+        <v>24.533586998993929</v>
       </c>
       <c r="AB11">
         <v>11.5623</v>
@@ -20936,35 +20936,35 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="7"/>
-        <v>28.715961305034224</v>
+        <v>30.512767946234984</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="8"/>
-        <v>21.187910772477252</v>
+        <v>18.780270113741288</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="9"/>
-        <v>28.728274830813668</v>
+        <v>30.145075335310359</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="10"/>
-        <v>86.223633624579534</v>
+        <v>87.491803613286578</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="11"/>
-        <v>86.223633624579534</v>
+        <v>87.491803613286578</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="12"/>
-        <v>28.728274830813668</v>
+        <v>30.145075335310359</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="13"/>
-        <v>21.187910772477252</v>
+        <v>18.780270113741288</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="14"/>
-        <v>24.95809280164546</v>
+        <v>24.462672724525824</v>
       </c>
       <c r="AB12">
         <v>5.7392000000000003</v>
@@ -21016,35 +21016,35 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="7"/>
-        <v>27.853837849400037</v>
+        <v>27.003195549398733</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="8"/>
-        <v>20.509306205081604</v>
+        <v>19.187155010159472</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="9"/>
-        <v>28.028725245682764</v>
+        <v>27.631571506581061</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="10"/>
-        <v>85.459533230531918</v>
+        <v>84.72731391074278</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="11"/>
-        <v>85.459533230531918</v>
+        <v>84.72731391074278</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="12"/>
-        <v>28.028725245682764</v>
+        <v>27.631571506581061</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="13"/>
-        <v>20.509306205081604</v>
+        <v>19.187155010159472</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="14"/>
-        <v>24.269015725382182</v>
+        <v>23.409363258370266</v>
       </c>
       <c r="AB13">
         <v>14.312900000000001</v>
@@ -21092,39 +21092,39 @@
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="7"/>
-        <v>32.381059896928669</v>
+        <v>17.243197351021319</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="8"/>
-        <v>17.257214847628202</v>
+        <v>14.522460471368635</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="9"/>
-        <v>31.510592966679489</v>
+        <v>19.320872182133268</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="10"/>
-        <v>86.516150103653771</v>
+        <v>42.986723412771944</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="11"/>
-        <v>86.516150103653771</v>
+        <v>51.675852824536648</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="12"/>
-        <v>31.510592966679489</v>
+        <v>19.320872182133268</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="13"/>
-        <v>17.257214847628202</v>
+        <v>14.522460471368635</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="14"/>
-        <v>24.383903907153844</v>
+        <v>16.921666326750952</v>
       </c>
       <c r="AB14">
         <v>12.5059</v>
@@ -21176,35 +21176,35 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="7"/>
-        <v>24.296040623717541</v>
+        <v>31.528575082222634</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="8"/>
-        <v>16.7947763832777</v>
+        <v>16.553644441058694</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="9"/>
-        <v>25.738951092309932</v>
+        <v>29.087034502204762</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="10"/>
-        <v>86.595876739797902</v>
+        <v>87.176621471075379</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="11"/>
-        <v>86.595876739797902</v>
+        <v>87.176621471075379</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="12"/>
-        <v>25.738951092309932</v>
+        <v>29.087034502204762</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="13"/>
-        <v>16.7947763832777</v>
+        <v>16.553644441058694</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="14"/>
-        <v>21.266863737793816</v>
+        <v>22.820339471631726</v>
       </c>
       <c r="AB15">
         <v>12.5343</v>
@@ -21256,35 +21256,35 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="7"/>
-        <v>26.977637231097731</v>
+        <v>25.492495712980482</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="8"/>
-        <v>18.771918912222858</v>
+        <v>15.240517004233212</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="9"/>
-        <v>26.72990000334017</v>
+        <v>26.211403470825342</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="10"/>
-        <v>90.375259727370832</v>
+        <v>90.435116104374529</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="11"/>
-        <v>90.375259727370832</v>
+        <v>90.435116104374529</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="12"/>
-        <v>26.72990000334017</v>
+        <v>26.211403470825342</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="13"/>
-        <v>18.771918912222858</v>
+        <v>15.240517004233212</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="14"/>
-        <v>22.750909457781514</v>
+        <v>20.725960237529279</v>
       </c>
       <c r="AB16">
         <v>10.6838</v>
@@ -21336,35 +21336,35 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="7"/>
-        <v>29.732412542709906</v>
+        <v>23.524062286953402</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="8"/>
-        <v>16.647184988744243</v>
+        <v>12.603060224198551</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="9"/>
-        <v>29.131910034835961</v>
+        <v>24.061530523727789</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="10"/>
-        <v>90.519681934767718</v>
+        <v>90.889902718555419</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="11"/>
-        <v>90.519681934767718</v>
+        <v>90.889902718555419</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="12"/>
-        <v>29.131910034835961</v>
+        <v>24.061530523727789</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="13"/>
-        <v>16.647184988744243</v>
+        <v>12.603060224198551</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="14"/>
-        <v>22.889547511790102</v>
+        <v>18.33229537396317</v>
       </c>
       <c r="AB17">
         <v>10.097799999999999</v>
@@ -21412,39 +21412,39 @@
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="7"/>
-        <v>20.540628973777892</v>
+        <v>25.622249690995979</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="8"/>
-        <v>16.326498623696317</v>
+        <v>15.08445549770784</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="9"/>
-        <v>22.258885185989509</v>
+        <v>25.310105857542343</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="10"/>
-        <v>46.038648974559322</v>
+        <v>92.396401778633063</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="11"/>
-        <v>55.294460739265205</v>
+        <v>92.396401778633063</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="12"/>
-        <v>22.258885185989509</v>
+        <v>25.310105857542343</v>
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="13"/>
-        <v>16.326498623696317</v>
+        <v>15.08445549770784</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="14"/>
-        <v>19.292691904842911</v>
+        <v>20.197280677625091</v>
       </c>
       <c r="AB18">
         <v>9.4130400000000005</v>
@@ -21492,39 +21492,39 @@
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="7"/>
-        <v>25.03974672692323</v>
+        <v>33.629874132407949</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="8"/>
-        <v>14.790588376920999</v>
+        <v>10.274496415490045</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="9"/>
-        <v>24.483574418736488</v>
+        <v>31.965920477434828</v>
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="10"/>
-        <v>43.536833332364289</v>
+        <v>88.92878956524028</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="11"/>
-        <v>52.414856861776059</v>
+        <v>88.92878956524028</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="12"/>
-        <v>24.483574418736488</v>
+        <v>31.965920477434828</v>
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="13"/>
-        <v>14.790588376920999</v>
+        <v>10.274496415490045</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="14"/>
-        <v>19.637081397828744</v>
+        <v>21.120208446462435</v>
       </c>
       <c r="AB19">
         <v>8.5562000000000005</v>
@@ -21576,35 +21576,35 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="7"/>
-        <v>24.844414674816981</v>
+        <v>24.512101351100803</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="8"/>
-        <v>13.647592625090283</v>
+        <v>14.245589611344045</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="9"/>
-        <v>24.772246623600882</v>
+        <v>26.00286517636761</v>
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="10"/>
-        <v>95.297216806581318</v>
+        <v>94.344816931383491</v>
       </c>
       <c r="P20">
         <f t="shared" ca="1" si="11"/>
-        <v>95.297216806581318</v>
+        <v>94.344816931383491</v>
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="12"/>
-        <v>24.772246623600882</v>
+        <v>26.00286517636761</v>
       </c>
       <c r="R20">
         <f t="shared" ca="1" si="13"/>
-        <v>13.647592625090283</v>
+        <v>14.245589611344045</v>
       </c>
       <c r="S20">
         <f t="shared" ca="1" si="14"/>
-        <v>19.209919624345581</v>
+        <v>20.124227393855826</v>
       </c>
       <c r="AB20">
         <v>7.9345800000000004</v>
@@ -21652,39 +21652,39 @@
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="7"/>
-        <v>23.553005174107465</v>
+        <v>25.974739184945978</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="8"/>
-        <v>13.517109086458346</v>
+        <v>19.167117909755781</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="9"/>
-        <v>23.796853464006148</v>
+        <v>25.980364383230306</v>
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="10"/>
-        <v>45.297975968785927</v>
+        <v>90.503750467150283</v>
       </c>
       <c r="P21">
         <f t="shared" ca="1" si="11"/>
-        <v>54.36489361584475</v>
+        <v>90.503750467150283</v>
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="12"/>
-        <v>23.796853464006148</v>
+        <v>25.980364383230306</v>
       </c>
       <c r="R21">
         <f t="shared" ca="1" si="13"/>
-        <v>13.517109086458346</v>
+        <v>19.167117909755781</v>
       </c>
       <c r="S21">
         <f t="shared" ca="1" si="14"/>
-        <v>18.656981275232248</v>
+        <v>22.573741146493042</v>
       </c>
       <c r="AB21">
         <v>15.4214</v>
@@ -21736,35 +21736,35 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="7"/>
-        <v>29.673248723678871</v>
+        <v>22.503242997124783</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="8"/>
-        <v>18.717095203175752</v>
+        <v>19.338634690717473</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="9"/>
-        <v>28.497969671744329</v>
+        <v>23.198667274345887</v>
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="10"/>
-        <v>94.12221143173619</v>
+        <v>94.748922842168326</v>
       </c>
       <c r="P22">
         <f t="shared" ca="1" si="11"/>
-        <v>94.12221143173619</v>
+        <v>94.748922842168326</v>
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="12"/>
-        <v>28.497969671744329</v>
+        <v>23.198667274345887</v>
       </c>
       <c r="R22">
         <f t="shared" ca="1" si="13"/>
-        <v>18.717095203175752</v>
+        <v>19.338634690717473</v>
       </c>
       <c r="S22">
         <f t="shared" ca="1" si="14"/>
-        <v>23.607532437460041</v>
+        <v>21.268650982531682</v>
       </c>
       <c r="AB22">
         <v>11.3246</v>
@@ -21812,39 +21812,39 @@
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="7"/>
-        <v>21.606312128786666</v>
+        <v>27.978835936763232</v>
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="8"/>
-        <v>18.524278372461524</v>
+        <v>16.552374345472636</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="9"/>
-        <v>22.984643637378198</v>
+        <v>27.022802204279763</v>
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="10"/>
-        <v>45.875949719701822</v>
+        <v>92.741841782295452</v>
       </c>
       <c r="P23">
         <f t="shared" ca="1" si="11"/>
-        <v>55.131761484407704</v>
+        <v>92.741841782295452</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="12"/>
-        <v>22.984643637378198</v>
+        <v>27.022802204279763</v>
       </c>
       <c r="R23">
         <f t="shared" ca="1" si="13"/>
-        <v>18.524278372461524</v>
+        <v>16.552374345472636</v>
       </c>
       <c r="S23">
         <f t="shared" ca="1" si="14"/>
-        <v>20.754461004919861</v>
+        <v>21.7875882748762</v>
       </c>
       <c r="AB23">
         <v>7.1011600000000001</v>
@@ -21896,35 +21896,35 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="7"/>
-        <v>27.483418742905489</v>
+        <v>23.207043685099663</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="8"/>
-        <v>20.71529030284762</v>
+        <v>15.096427487120485</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="9"/>
-        <v>26.583663721800033</v>
+        <v>23.970195388935682</v>
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="10"/>
-        <v>92.607262176590794</v>
+        <v>92.471995593560422</v>
       </c>
       <c r="P24">
         <f t="shared" ca="1" si="11"/>
-        <v>92.607262176590794</v>
+        <v>92.471995593560422</v>
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="12"/>
-        <v>26.583663721800033</v>
+        <v>23.970195388935682</v>
       </c>
       <c r="R24">
         <f t="shared" ca="1" si="13"/>
-        <v>20.71529030284762</v>
+        <v>15.096427487120485</v>
       </c>
       <c r="S24">
         <f t="shared" ca="1" si="14"/>
-        <v>23.649477012323828</v>
+        <v>19.533311438028083</v>
       </c>
       <c r="AB24">
         <v>11.790699999999999</v>
@@ -21972,39 +21972,39 @@
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="7"/>
-        <v>27.844125206326009</v>
+        <v>24.407552885379335</v>
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="8"/>
-        <v>19.474879279340399</v>
+        <v>17.083125420105304</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="9"/>
-        <v>27.592032909420816</v>
+        <v>24.320081386090607</v>
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="10"/>
-        <v>94.207115903211161</v>
+        <v>47.129289132197414</v>
       </c>
       <c r="P25">
         <f t="shared" ca="1" si="11"/>
-        <v>94.207115903211161</v>
+        <v>56.573995014550356</v>
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="12"/>
-        <v>27.592032909420816</v>
+        <v>24.320081386090607</v>
       </c>
       <c r="R25">
         <f t="shared" ca="1" si="13"/>
-        <v>19.474879279340399</v>
+        <v>17.083125420105304</v>
       </c>
       <c r="S25">
         <f t="shared" ca="1" si="14"/>
-        <v>23.533456094380607</v>
+        <v>20.701603403097955</v>
       </c>
       <c r="AB25">
         <v>7.1720600000000001</v>
@@ -22052,39 +22052,39 @@
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="7"/>
-        <v>32.588939842286827</v>
+        <v>26.592403891638881</v>
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="8"/>
-        <v>12.774441542397964</v>
+        <v>15.291077759443521</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="9"/>
-        <v>31.589558455713629</v>
+        <v>26.137939390529226</v>
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="10"/>
-        <v>91.935005122360849</v>
+        <v>46.083081819018801</v>
       </c>
       <c r="P26">
         <f t="shared" ca="1" si="11"/>
-        <v>91.935005122360849</v>
+        <v>55.338893583724683</v>
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="12"/>
-        <v>31.589558455713629</v>
+        <v>26.137939390529226</v>
       </c>
       <c r="R26">
         <f t="shared" ca="1" si="13"/>
-        <v>12.774441542397964</v>
+        <v>15.291077759443521</v>
       </c>
       <c r="S26">
         <f t="shared" ca="1" si="14"/>
-        <v>22.181999999055797</v>
+        <v>20.714508574986375</v>
       </c>
       <c r="AB26">
         <v>11.055199999999999</v>
@@ -22132,39 +22132,39 @@
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="7"/>
-        <v>20.04140286628018</v>
+        <v>22.63781131462844</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="8"/>
-        <v>16.201720618556866</v>
+        <v>12.371485891951234</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="9"/>
-        <v>22.351033984166872</v>
+        <v>23.337836929808596</v>
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="10"/>
-        <v>44.192833903096769</v>
+        <v>88.475238227270992</v>
       </c>
       <c r="P27">
         <f t="shared" ca="1" si="11"/>
-        <v>53.070857432508532</v>
+        <v>88.475238227270992</v>
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="12"/>
-        <v>22.351033984166872</v>
+        <v>23.337836929808596</v>
       </c>
       <c r="R27">
         <f t="shared" ca="1" si="13"/>
-        <v>16.201720618556866</v>
+        <v>12.371485891951234</v>
       </c>
       <c r="S27">
         <f t="shared" ca="1" si="14"/>
-        <v>19.276377301361869</v>
+        <v>17.854661410879913</v>
       </c>
       <c r="AB27">
         <v>5.6329700000000003</v>
@@ -22212,39 +22212,39 @@
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="7"/>
-        <v>23.455323184482378</v>
+        <v>26.558657504378022</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="8"/>
-        <v>12.634186534345524</v>
+        <v>17.464792035564781</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="9"/>
-        <v>23.234465344419277</v>
+        <v>25.914493389464141</v>
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="10"/>
-        <v>44.911533440695862</v>
+        <v>90.459632769749092</v>
       </c>
       <c r="P28">
         <f t="shared" ca="1" si="11"/>
-        <v>53.978451087754685</v>
+        <v>90.459632769749092</v>
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="12"/>
-        <v>23.234465344419277</v>
+        <v>25.914493389464141</v>
       </c>
       <c r="R28">
         <f t="shared" ca="1" si="13"/>
-        <v>12.634186534345524</v>
+        <v>17.464792035564781</v>
       </c>
       <c r="S28">
         <f t="shared" ca="1" si="14"/>
-        <v>17.934325939382401</v>
+        <v>21.689642712514463</v>
       </c>
       <c r="AB28">
         <v>4.3788200000000002</v>
@@ -22296,35 +22296,35 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="7"/>
-        <v>24.77785586168158</v>
+        <v>28.127590415883979</v>
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="8"/>
-        <v>15.112027072439044</v>
+        <v>11.973883633289953</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="9"/>
-        <v>24.469177758229122</v>
+        <v>27.684971010600016</v>
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="10"/>
-        <v>91.076865674527227</v>
+        <v>91.124527115754532</v>
       </c>
       <c r="P29">
         <f t="shared" ca="1" si="11"/>
-        <v>91.076865674527227</v>
+        <v>91.124527115754532</v>
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="12"/>
-        <v>24.469177758229122</v>
+        <v>27.684971010600016</v>
       </c>
       <c r="R29">
         <f t="shared" ca="1" si="13"/>
-        <v>15.112027072439044</v>
+        <v>11.973883633289953</v>
       </c>
       <c r="S29">
         <f t="shared" ca="1" si="14"/>
-        <v>19.790602415334085</v>
+        <v>19.829427321944983</v>
       </c>
       <c r="AB29">
         <v>7.12798</v>
@@ -22376,35 +22376,35 @@
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="7"/>
-        <v>26.619187840122468</v>
+        <v>22.783142049041256</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="8"/>
-        <v>10.996984679591822</v>
+        <v>20.625141346192805</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="9"/>
-        <v>26.189185823743802</v>
+        <v>23.763507841353007</v>
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="10"/>
-        <v>86.460776735612825</v>
+        <v>87.322885627599717</v>
       </c>
       <c r="P30">
         <f t="shared" ca="1" si="11"/>
-        <v>86.460776735612825</v>
+        <v>87.322885627599717</v>
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="12"/>
-        <v>26.189185823743802</v>
+        <v>23.763507841353007</v>
       </c>
       <c r="R30">
         <f t="shared" ca="1" si="13"/>
-        <v>10.996984679591822</v>
+        <v>20.625141346192805</v>
       </c>
       <c r="S30">
         <f t="shared" ca="1" si="14"/>
-        <v>18.593085251667812</v>
+        <v>22.194324593772905</v>
       </c>
       <c r="AB30">
         <v>3.10764</v>
@@ -22456,35 +22456,35 @@
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="7"/>
-        <v>29.153239606802373</v>
+        <v>27.046984976072569</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="8"/>
-        <v>14.728821539318091</v>
+        <v>13.646789583005873</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="9"/>
-        <v>28.560428850190661</v>
+        <v>26.39028954912866</v>
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="10"/>
-        <v>88.757132702114163</v>
+        <v>88.136555721268451</v>
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="11"/>
-        <v>88.757132702114163</v>
+        <v>88.136555721268451</v>
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="12"/>
-        <v>28.560428850190661</v>
+        <v>26.39028954912866</v>
       </c>
       <c r="R31">
         <f t="shared" ca="1" si="13"/>
-        <v>14.728821539318091</v>
+        <v>13.646789583005873</v>
       </c>
       <c r="S31">
         <f t="shared" ca="1" si="14"/>
-        <v>21.644625194754376</v>
+        <v>20.018539566067268</v>
       </c>
       <c r="AB31">
         <v>11.0318</v>
@@ -22536,35 +22536,35 @@
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="7"/>
-        <v>20.329509874936363</v>
+        <v>26.579549053365149</v>
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="8"/>
-        <v>8.7474648244060909</v>
+        <v>14.753841207099613</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="9"/>
-        <v>21.975693669987223</v>
+        <v>26.541697152517855</v>
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="10"/>
-        <v>89.294092413167022</v>
+        <v>89.274029588135974</v>
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="11"/>
-        <v>89.294092413167022</v>
+        <v>89.274029588135974</v>
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="12"/>
-        <v>21.975693669987223</v>
+        <v>26.541697152517855</v>
       </c>
       <c r="R32">
         <f t="shared" ca="1" si="13"/>
-        <v>8.7474648244060909</v>
+        <v>14.753841207099613</v>
       </c>
       <c r="S32">
         <f t="shared" ca="1" si="14"/>
-        <v>15.361579247196657</v>
+        <v>20.647769179808733</v>
       </c>
       <c r="AB32">
         <v>1.65354</v>
@@ -22631,35 +22631,35 @@
       </c>
       <c r="K34">
         <f ca="1">COUNTIF(K3:K33,"&gt;0")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L34" s="4">
         <f ca="1">AVERAGE(L3:L32)</f>
-        <v>26.732655762878444</v>
+        <v>26.398923516113783</v>
       </c>
       <c r="M34" s="4">
         <f ca="1">AVERAGE(M3:M32)</f>
-        <v>17.381533859832054</v>
+        <v>16.683531301314339</v>
       </c>
       <c r="N34" s="4">
         <f ca="1">AVERAGE(N3:N32)</f>
-        <v>26.819264162767347</v>
+        <v>26.422050394024613</v>
       </c>
       <c r="O34" s="4">
         <f ca="1">AVERAGE(O3:O32)</f>
-        <v>81.023136083213572</v>
+        <v>85.901346652646282</v>
       </c>
       <c r="Q34" s="8">
         <f ca="1">AVERAGE(Q3:Q32)</f>
-        <v>26.819264162767347</v>
+        <v>26.422050394024613</v>
       </c>
       <c r="R34" s="8">
         <f ca="1">AVERAGE(R3:R32)</f>
-        <v>17.381533859832054</v>
+        <v>16.683531301314339</v>
       </c>
       <c r="S34">
         <f ca="1">AVERAGE(S3:S32)</f>
-        <v>22.100399011299704</v>
+        <v>21.552790847669474</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
@@ -22686,27 +22686,27 @@
       </c>
       <c r="L35">
         <f ca="1">_xlfn.STDEV.P(L3:L32)</f>
-        <v>3.4092748808747508</v>
+        <v>3.6128488203798286</v>
       </c>
       <c r="M35">
         <f t="shared" ref="M35:N35" ca="1" si="18">_xlfn.STDEV.P(M3:M32)</f>
-        <v>3.704663997251493</v>
+        <v>2.8328034300141529</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="18"/>
-        <v>2.797867479856524</v>
+        <v>2.8834525112984024</v>
       </c>
       <c r="O35">
         <f t="shared" ref="O35" ca="1" si="19">_xlfn.STDEV.P(O3:O32)</f>
-        <v>21.807606410371513</v>
+        <v>19.424174914917423</v>
       </c>
       <c r="Q35">
         <f ca="1">_xlfn.STDEV.P(Q3:Q32)</f>
-        <v>2.797867479856524</v>
+        <v>2.8834525112984024</v>
       </c>
       <c r="R35">
         <f ca="1">_xlfn.STDEV.P(R3:R32)</f>
-        <v>3.704663997251493</v>
+        <v>2.8328034300141529</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
@@ -35088,7 +35088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed "scratchpaper" files. Coding dormancy
The REG scratchpaper file was removed among others.
</commit_message>
<xml_diff>
--- a/Design docs/sunlightstats.xlsx
+++ b/Design docs/sunlightstats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="25875" windowHeight="11370"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="25875" windowHeight="11370" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="raws" sheetId="1" r:id="rId1"/>
@@ -833,94 +833,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>29.316922501816855</c:v>
+                  <c:v>32.368701656654501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.97904619475829</c:v>
+                  <c:v>29.391405596902064</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.031892208565473</c:v>
+                  <c:v>27.861720334803287</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.809197646081287</c:v>
+                  <c:v>30.117052544330104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.690601511623402</c:v>
+                  <c:v>26.715127698019575</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.65888301636889</c:v>
+                  <c:v>26.479623961825599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.514219844190961</c:v>
+                  <c:v>27.861775571505913</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.987219073310218</c:v>
+                  <c:v>25.797220892258956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.674304891611857</c:v>
+                  <c:v>28.777528933931428</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.145075335310359</c:v>
+                  <c:v>28.728274830813668</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.631571506581061</c:v>
+                  <c:v>28.028725245682764</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.320872182133268</c:v>
+                  <c:v>31.510592966679489</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.087034502204762</c:v>
+                  <c:v>25.738951092309932</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.211403470825342</c:v>
+                  <c:v>26.72990000334017</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.061530523727789</c:v>
+                  <c:v>29.131910034835961</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25.310105857542343</c:v>
+                  <c:v>22.258885185989509</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31.965920477434828</c:v>
+                  <c:v>24.483574418736488</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26.00286517636761</c:v>
+                  <c:v>24.772246623600882</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25.980364383230306</c:v>
+                  <c:v>23.796853464006148</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23.198667274345887</c:v>
+                  <c:v>28.497969671744329</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27.022802204279763</c:v>
+                  <c:v>22.984643637378198</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23.970195388935682</c:v>
+                  <c:v>26.583663721800033</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>24.320081386090607</c:v>
+                  <c:v>27.592032909420816</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>26.137939390529226</c:v>
+                  <c:v>31.589558455713629</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23.337836929808596</c:v>
+                  <c:v>22.351033984166872</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.914493389464141</c:v>
+                  <c:v>23.234465344419277</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27.684971010600016</c:v>
+                  <c:v>24.469177758229122</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>23.763507841353007</c:v>
+                  <c:v>26.189185823743802</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>26.39028954912866</c:v>
+                  <c:v>28.560428850190661</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>26.541697152517855</c:v>
+                  <c:v>21.975693669987223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,94 +956,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>16.859712771399856</c:v>
+                  <c:v>25.215260395062391</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.814460679903792</c:v>
+                  <c:v>22.145668079642252</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.594292517835736</c:v>
+                  <c:v>18.359330345228397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.195241280878182</c:v>
+                  <c:v>18.269011418315554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.752612739860062</c:v>
+                  <c:v>23.520157241313434</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.627524019215297</c:v>
+                  <c:v>22.933491370605889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.073494649460251</c:v>
+                  <c:v>17.338926267049509</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.339391175479683</c:v>
+                  <c:v>16.784268409265042</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.392869106376001</c:v>
+                  <c:v>18.802611478000724</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.780270113741288</c:v>
+                  <c:v>21.187910772477252</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.187155010159472</c:v>
+                  <c:v>20.509306205081604</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.522460471368635</c:v>
+                  <c:v>17.257214847628202</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.553644441058694</c:v>
+                  <c:v>16.7947763832777</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15.240517004233212</c:v>
+                  <c:v>18.771918912222858</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.603060224198551</c:v>
+                  <c:v>16.647184988744243</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.08445549770784</c:v>
+                  <c:v>16.326498623696317</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.274496415490045</c:v>
+                  <c:v>14.790588376920999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.245589611344045</c:v>
+                  <c:v>13.647592625090283</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.167117909755781</c:v>
+                  <c:v>13.517109086458346</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.338634690717473</c:v>
+                  <c:v>18.717095203175752</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.552374345472636</c:v>
+                  <c:v>18.524278372461524</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15.096427487120485</c:v>
+                  <c:v>20.71529030284762</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>17.083125420105304</c:v>
+                  <c:v>19.474879279340399</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15.291077759443521</c:v>
+                  <c:v>12.774441542397964</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.371485891951234</c:v>
+                  <c:v>16.201720618556866</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17.464792035564781</c:v>
+                  <c:v>12.634186534345524</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.973883633289953</c:v>
+                  <c:v>15.112027072439044</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20.625141346192805</c:v>
+                  <c:v>10.996984679591822</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.646789583005873</c:v>
+                  <c:v>14.728821539318091</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14.753841207099613</c:v>
+                  <c:v>8.7474648244060909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,11 +1060,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174414336"/>
-        <c:axId val="146639680"/>
+        <c:axId val="184179200"/>
+        <c:axId val="166497088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174414336"/>
+        <c:axId val="184179200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1073,7 +1073,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146639680"/>
+        <c:crossAx val="166497088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1081,7 +1081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146639680"/>
+        <c:axId val="166497088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1111,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174414336"/>
+        <c:crossAx val="184179200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1398,11 +1398,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174698496"/>
-        <c:axId val="146641984"/>
+        <c:axId val="184463360"/>
+        <c:axId val="166499392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174698496"/>
+        <c:axId val="184463360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146641984"/>
+        <c:crossAx val="166499392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146641984"/>
+        <c:axId val="166499392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174698496"/>
+        <c:crossAx val="184463360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1484,94 +1484,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>111.3098112466526</c:v>
+                  <c:v>111.84024915523568</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107.34284984908234</c:v>
+                  <c:v>54.847910366204488</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109.52907121528061</c:v>
+                  <c:v>109.74333356427809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.36398978595108</c:v>
+                  <c:v>110.41095666046003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.46519993019399</c:v>
+                  <c:v>103.66801115994332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99.696449699729357</c:v>
+                  <c:v>49.628544443785216</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47.275334596998661</c:v>
+                  <c:v>94.948822284544448</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44.114678007454344</c:v>
+                  <c:v>89.069305904418229</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.093775055812671</c:v>
+                  <c:v>87.235359291730873</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>87.491803613286578</c:v>
+                  <c:v>86.223633624579534</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.72731391074278</c:v>
+                  <c:v>85.459533230531918</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.986723412771944</c:v>
+                  <c:v>86.516150103653771</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>87.176621471075379</c:v>
+                  <c:v>86.595876739797902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90.435116104374529</c:v>
+                  <c:v>90.375259727370832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90.889902718555419</c:v>
+                  <c:v>90.519681934767718</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.396401778633063</c:v>
+                  <c:v>46.038648974559322</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>88.92878956524028</c:v>
+                  <c:v>43.536833332364289</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>94.344816931383491</c:v>
+                  <c:v>95.297216806581318</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90.503750467150283</c:v>
+                  <c:v>45.297975968785927</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>94.748922842168326</c:v>
+                  <c:v>94.12221143173619</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>92.741841782295452</c:v>
+                  <c:v>45.875949719701822</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>92.471995593560422</c:v>
+                  <c:v>92.607262176590794</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>47.129289132197414</c:v>
+                  <c:v>94.207115903211161</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>46.083081819018801</c:v>
+                  <c:v>91.935005122360849</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>88.475238227270992</c:v>
+                  <c:v>44.192833903096769</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>90.459632769749092</c:v>
+                  <c:v>44.911533440695862</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>91.124527115754532</c:v>
+                  <c:v>91.076865674527227</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>87.322885627599717</c:v>
+                  <c:v>86.460776735612825</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>88.136555721268451</c:v>
+                  <c:v>88.757132702114163</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>89.274029588135974</c:v>
+                  <c:v>89.294092413167022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1591,94 +1591,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>111.3098112466526</c:v>
+                  <c:v>111.84024915523568</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107.34284984908234</c:v>
+                  <c:v>65.614875072086846</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109.52907121528061</c:v>
+                  <c:v>109.74333356427809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.36398978595108</c:v>
+                  <c:v>110.41095666046003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.46519993019399</c:v>
+                  <c:v>103.66801115994332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99.696449699729357</c:v>
+                  <c:v>59.639932679079337</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.720040479351603</c:v>
+                  <c:v>94.948822284544448</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52.992701536866107</c:v>
+                  <c:v>89.069305904418229</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.093775055812671</c:v>
+                  <c:v>87.235359291730873</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>87.491803613286578</c:v>
+                  <c:v>86.223633624579534</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.72731391074278</c:v>
+                  <c:v>85.459533230531918</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51.675852824536648</c:v>
+                  <c:v>86.516150103653771</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>87.176621471075379</c:v>
+                  <c:v>86.595876739797902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90.435116104374529</c:v>
+                  <c:v>90.375259727370832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90.889902718555419</c:v>
+                  <c:v>90.519681934767718</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.396401778633063</c:v>
+                  <c:v>55.294460739265205</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>88.92878956524028</c:v>
+                  <c:v>52.414856861776059</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>94.344816931383491</c:v>
+                  <c:v>95.297216806581318</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90.503750467150283</c:v>
+                  <c:v>54.36489361584475</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>94.748922842168326</c:v>
+                  <c:v>94.12221143173619</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>92.741841782295452</c:v>
+                  <c:v>55.131761484407704</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>92.471995593560422</c:v>
+                  <c:v>92.607262176590794</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>56.573995014550356</c:v>
+                  <c:v>94.207115903211161</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>55.338893583724683</c:v>
+                  <c:v>91.935005122360849</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>88.475238227270992</c:v>
+                  <c:v>53.070857432508532</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>90.459632769749092</c:v>
+                  <c:v>53.978451087754685</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>91.124527115754532</c:v>
+                  <c:v>91.076865674527227</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>87.322885627599717</c:v>
+                  <c:v>86.460776735612825</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>88.136555721268451</c:v>
+                  <c:v>88.757132702114163</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>89.274029588135974</c:v>
+                  <c:v>89.294092413167022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1695,11 +1695,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174700032"/>
-        <c:axId val="146643712"/>
+        <c:axId val="184464896"/>
+        <c:axId val="166501120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174700032"/>
+        <c:axId val="184464896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146643712"/>
+        <c:crossAx val="166501120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +1716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146643712"/>
+        <c:axId val="166501120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174700032"/>
+        <c:crossAx val="184464896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2895,11 +2895,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="174700544"/>
-        <c:axId val="194060864"/>
+        <c:axId val="184465408"/>
+        <c:axId val="191242816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="174700544"/>
+        <c:axId val="184465408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2908,7 +2908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194060864"/>
+        <c:crossAx val="191242816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2916,7 +2916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194060864"/>
+        <c:axId val="191242816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2927,7 +2927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174700544"/>
+        <c:crossAx val="184465408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4071,8 +4071,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="174702080"/>
-        <c:axId val="194062592"/>
+        <c:axId val="184466944"/>
+        <c:axId val="191244544"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6279,11 +6279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182870528"/>
-        <c:axId val="194063168"/>
+        <c:axId val="191119872"/>
+        <c:axId val="191245120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174702080"/>
+        <c:axId val="184466944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6292,7 +6292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194062592"/>
+        <c:crossAx val="191244544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6300,7 +6300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194062592"/>
+        <c:axId val="191244544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6311,12 +6311,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174702080"/>
+        <c:crossAx val="184466944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194063168"/>
+        <c:axId val="191245120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6326,12 +6326,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182870528"/>
+        <c:crossAx val="191119872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="182870528"/>
+        <c:axId val="191119872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6340,7 +6340,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194063168"/>
+        <c:crossAx val="191245120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7520,8 +7520,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182872576"/>
-        <c:axId val="194066048"/>
+        <c:axId val="191121920"/>
+        <c:axId val="191248000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9788,11 +9788,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182871552"/>
-        <c:axId val="194065472"/>
+        <c:axId val="191120896"/>
+        <c:axId val="191247424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="182871552"/>
+        <c:axId val="191120896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9801,7 +9801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194065472"/>
+        <c:crossAx val="191247424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9809,7 +9809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194065472"/>
+        <c:axId val="191247424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9820,12 +9820,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182871552"/>
+        <c:crossAx val="191120896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194066048"/>
+        <c:axId val="191248000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9835,12 +9835,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182872576"/>
+        <c:crossAx val="191121920"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="182872576"/>
+        <c:axId val="191121920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9849,7 +9849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194066048"/>
+        <c:crossAx val="191248000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11035,11 +11035,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182873088"/>
-        <c:axId val="194412544"/>
+        <c:axId val="191122432"/>
+        <c:axId val="191594496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182873088"/>
+        <c:axId val="191122432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11048,7 +11048,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194412544"/>
+        <c:crossAx val="191594496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11056,7 +11056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194412544"/>
+        <c:axId val="191594496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11067,7 +11067,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182873088"/>
+        <c:crossAx val="191122432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13343,8 +13343,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="194414272"/>
-        <c:axId val="194414848"/>
+        <c:axId val="191596224"/>
+        <c:axId val="191596800"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -15584,11 +15584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="194416000"/>
-        <c:axId val="194415424"/>
+        <c:axId val="191597952"/>
+        <c:axId val="191597376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="194414272"/>
+        <c:axId val="191596224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15598,12 +15598,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194414848"/>
+        <c:crossAx val="191596800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194414848"/>
+        <c:axId val="191596800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15614,12 +15614,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194414272"/>
+        <c:crossAx val="191596224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194415424"/>
+        <c:axId val="191597376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15629,12 +15629,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194416000"/>
+        <c:crossAx val="191597952"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194416000"/>
+        <c:axId val="191597952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15644,7 +15644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194415424"/>
+        <c:crossAx val="191597376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16212,7 +16212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -20216,35 +20216,35 @@
       </c>
       <c r="L3">
         <f ca="1">_xlfn.NORM.INV(RAND(), IF(K3=1,E3,F3), $B$35)</f>
-        <v>29.316922501816855</v>
+        <v>32.368701656654501</v>
       </c>
       <c r="M3">
         <f ca="1">_xlfn.NORM.INV(RAND(), G3, $C$35/3)</f>
-        <v>16.859712771399856</v>
+        <v>25.215260395062391</v>
       </c>
       <c r="N3">
         <f ca="1">L3</f>
-        <v>29.316922501816855</v>
+        <v>32.368701656654501</v>
       </c>
       <c r="O3">
         <f ca="1">_xlfn.NORM.INV(RAND(), IF(K3=1,J3,I3), $D$35)</f>
-        <v>111.3098112466526</v>
+        <v>111.84024915523568</v>
       </c>
       <c r="P3">
         <f ca="1">IF(K3=1, O3 + 0.1 * I3, O3)</f>
-        <v>111.3098112466526</v>
+        <v>111.84024915523568</v>
       </c>
       <c r="Q3">
         <f ca="1">IF(N3 &lt; M3, M3, N3)</f>
-        <v>29.316922501816855</v>
+        <v>32.368701656654501</v>
       </c>
       <c r="R3">
         <f ca="1">IF(N3 &lt; M3, N3, M3)</f>
-        <v>16.859712771399856</v>
+        <v>25.215260395062391</v>
       </c>
       <c r="S3">
         <f ca="1">AVERAGE(Q3,R3)</f>
-        <v>23.088317636608355</v>
+        <v>28.791981025858448</v>
       </c>
       <c r="AB3">
         <v>12.581799999999999</v>
@@ -20292,39 +20292,39 @@
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L32" ca="1" si="7">_xlfn.NORM.INV(RAND(), IF(K4=1,E4,F4), $B$35)</f>
-        <v>31.394577117993649</v>
+        <v>28.647081581963953</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M32" ca="1" si="8">_xlfn.NORM.INV(RAND(), G4, $C$35/3)</f>
-        <v>18.814460679903792</v>
+        <v>22.145668079642252</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N32" ca="1" si="9">N3 * $N$1 + (1-$N$1) * L4</f>
-        <v>30.97904619475829</v>
+        <v>29.391405596902064</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O32" ca="1" si="10">_xlfn.NORM.INV(RAND(), IF(K4=1,J4,I4), $D$35)</f>
-        <v>107.34284984908234</v>
+        <v>54.847910366204488</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P32" ca="1" si="11">IF(K4=1, O4 + 0.1 * I4, O4)</f>
-        <v>107.34284984908234</v>
+        <v>65.614875072086846</v>
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q32" ca="1" si="12">IF(N4 &lt; M4, M4, N4)</f>
-        <v>30.97904619475829</v>
+        <v>29.391405596902064</v>
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R32" ca="1" si="13">IF(N4 &lt; M4, N4, M4)</f>
-        <v>18.814460679903792</v>
+        <v>22.145668079642252</v>
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S32" ca="1" si="14">AVERAGE(Q4,R4)</f>
-        <v>24.896753437331043</v>
+        <v>25.768536838272158</v>
       </c>
       <c r="AB4">
         <v>8.5861499999999999</v>
@@ -20376,35 +20376,35 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="7"/>
-        <v>29.795103712017269</v>
+        <v>27.479299019278589</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="8"/>
-        <v>17.594292517835736</v>
+        <v>18.359330345228397</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="9"/>
-        <v>30.031892208565473</v>
+        <v>27.861720334803287</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="10"/>
-        <v>109.52907121528061</v>
+        <v>109.74333356427809</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="11"/>
-        <v>109.52907121528061</v>
+        <v>109.74333356427809</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="12"/>
-        <v>30.031892208565473</v>
+        <v>27.861720334803287</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="13"/>
-        <v>17.594292517835736</v>
+        <v>18.359330345228397</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="14"/>
-        <v>23.813092363200603</v>
+        <v>23.11052534001584</v>
       </c>
       <c r="AB5">
         <v>22.792100000000001</v>
@@ -20456,35 +20456,35 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="7"/>
-        <v>26.003524005460239</v>
+        <v>30.680885596711807</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="8"/>
-        <v>19.195241280878182</v>
+        <v>18.269011418315554</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="9"/>
-        <v>26.809197646081287</v>
+        <v>30.117052544330104</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="10"/>
-        <v>109.36398978595108</v>
+        <v>110.41095666046003</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="11"/>
-        <v>109.36398978595108</v>
+        <v>110.41095666046003</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="12"/>
-        <v>26.809197646081287</v>
+        <v>30.117052544330104</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="13"/>
-        <v>19.195241280878182</v>
+        <v>18.269011418315554</v>
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="14"/>
-        <v>23.002219463479733</v>
+        <v>24.193031981322829</v>
       </c>
       <c r="AB6">
         <v>15.0762</v>
@@ -20536,35 +20536,35 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="7"/>
-        <v>29.16095247800893</v>
+        <v>25.864646486441941</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="8"/>
-        <v>20.752612739860062</v>
+        <v>23.520157241313434</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="9"/>
-        <v>28.690601511623402</v>
+        <v>26.715127698019575</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="10"/>
-        <v>103.46519993019399</v>
+        <v>103.66801115994332</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="11"/>
-        <v>103.46519993019399</v>
+        <v>103.66801115994332</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="12"/>
-        <v>28.690601511623402</v>
+        <v>26.715127698019575</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="13"/>
-        <v>20.752612739860062</v>
+        <v>23.520157241313434</v>
       </c>
       <c r="S7">
         <f t="shared" ca="1" si="14"/>
-        <v>24.721607125741734</v>
+        <v>25.117642469666507</v>
       </c>
       <c r="AB7">
         <v>11.031000000000001</v>
@@ -20612,39 +20612,39 @@
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="7"/>
-        <v>29.900953392555259</v>
+        <v>26.420748027777105</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="8"/>
-        <v>21.627524019215297</v>
+        <v>22.933491370605889</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="9"/>
-        <v>29.65888301636889</v>
+        <v>26.479623961825599</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="10"/>
-        <v>99.696449699729357</v>
+        <v>49.628544443785216</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="11"/>
-        <v>99.696449699729357</v>
+        <v>59.639932679079337</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="12"/>
-        <v>29.65888301636889</v>
+        <v>26.479623961825599</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="13"/>
-        <v>21.627524019215297</v>
+        <v>22.933491370605889</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="14"/>
-        <v>25.643203517792095</v>
+        <v>24.706557666215744</v>
       </c>
       <c r="AB8">
         <v>4.3186200000000001</v>
@@ -20692,39 +20692,39 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="7"/>
-        <v>19.478054051146476</v>
+        <v>28.207313473925989</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="8"/>
-        <v>17.073494649460251</v>
+        <v>17.338926267049509</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="9"/>
-        <v>21.514219844190961</v>
+        <v>27.861775571505913</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="10"/>
-        <v>47.275334596998661</v>
+        <v>94.948822284544448</v>
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="11"/>
-        <v>56.720040479351603</v>
+        <v>94.948822284544448</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="12"/>
-        <v>21.514219844190961</v>
+        <v>27.861775571505913</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="13"/>
-        <v>17.073494649460251</v>
+        <v>17.338926267049509</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="14"/>
-        <v>19.293857246825606</v>
+        <v>22.600350919277709</v>
       </c>
       <c r="AB9">
         <v>14.938499999999999</v>
@@ -20772,39 +20772,39 @@
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="7"/>
-        <v>23.355468880590031</v>
+        <v>25.281082222447218</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="8"/>
-        <v>18.339391175479683</v>
+        <v>16.784268409265042</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="9"/>
-        <v>22.987219073310218</v>
+        <v>25.797220892258956</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="10"/>
-        <v>44.114678007454344</v>
+        <v>89.069305904418229</v>
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="11"/>
-        <v>52.992701536866107</v>
+        <v>89.069305904418229</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="12"/>
-        <v>22.987219073310218</v>
+        <v>25.797220892258956</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="13"/>
-        <v>18.339391175479683</v>
+        <v>16.784268409265042</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="14"/>
-        <v>20.663305124394952</v>
+        <v>21.290744650762001</v>
       </c>
       <c r="AB10">
         <v>18.5778</v>
@@ -20856,35 +20856,35 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="7"/>
-        <v>30.096076346187267</v>
+        <v>29.522605944349543</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="8"/>
-        <v>20.392869106376001</v>
+        <v>18.802611478000724</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="9"/>
-        <v>28.674304891611857</v>
+        <v>28.777528933931428</v>
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="10"/>
-        <v>87.093775055812671</v>
+        <v>87.235359291730873</v>
       </c>
       <c r="P11">
         <f t="shared" ca="1" si="11"/>
-        <v>87.093775055812671</v>
+        <v>87.235359291730873</v>
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="12"/>
-        <v>28.674304891611857</v>
+        <v>28.777528933931428</v>
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="13"/>
-        <v>20.392869106376001</v>
+        <v>18.802611478000724</v>
       </c>
       <c r="S11">
         <f t="shared" ca="1" si="14"/>
-        <v>24.533586998993929</v>
+        <v>23.790070205966074</v>
       </c>
       <c r="AB11">
         <v>11.5623</v>
@@ -20936,35 +20936,35 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="7"/>
-        <v>30.512767946234984</v>
+        <v>28.715961305034224</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="8"/>
-        <v>18.780270113741288</v>
+        <v>21.187910772477252</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="9"/>
-        <v>30.145075335310359</v>
+        <v>28.728274830813668</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="10"/>
-        <v>87.491803613286578</v>
+        <v>86.223633624579534</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="11"/>
-        <v>87.491803613286578</v>
+        <v>86.223633624579534</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="12"/>
-        <v>30.145075335310359</v>
+        <v>28.728274830813668</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="13"/>
-        <v>18.780270113741288</v>
+        <v>21.187910772477252</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="14"/>
-        <v>24.462672724525824</v>
+        <v>24.95809280164546</v>
       </c>
       <c r="AB12">
         <v>5.7392000000000003</v>
@@ -21016,35 +21016,35 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="7"/>
-        <v>27.003195549398733</v>
+        <v>27.853837849400037</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="8"/>
-        <v>19.187155010159472</v>
+        <v>20.509306205081604</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="9"/>
-        <v>27.631571506581061</v>
+        <v>28.028725245682764</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="10"/>
-        <v>84.72731391074278</v>
+        <v>85.459533230531918</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="11"/>
-        <v>84.72731391074278</v>
+        <v>85.459533230531918</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="12"/>
-        <v>27.631571506581061</v>
+        <v>28.028725245682764</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="13"/>
-        <v>19.187155010159472</v>
+        <v>20.509306205081604</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="14"/>
-        <v>23.409363258370266</v>
+        <v>24.269015725382182</v>
       </c>
       <c r="AB13">
         <v>14.312900000000001</v>
@@ -21092,39 +21092,39 @@
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="7"/>
-        <v>17.243197351021319</v>
+        <v>32.381059896928669</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="8"/>
-        <v>14.522460471368635</v>
+        <v>17.257214847628202</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="9"/>
-        <v>19.320872182133268</v>
+        <v>31.510592966679489</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="10"/>
-        <v>42.986723412771944</v>
+        <v>86.516150103653771</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="11"/>
-        <v>51.675852824536648</v>
+        <v>86.516150103653771</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="12"/>
-        <v>19.320872182133268</v>
+        <v>31.510592966679489</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="13"/>
-        <v>14.522460471368635</v>
+        <v>17.257214847628202</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="14"/>
-        <v>16.921666326750952</v>
+        <v>24.383903907153844</v>
       </c>
       <c r="AB14">
         <v>12.5059</v>
@@ -21176,35 +21176,35 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="7"/>
-        <v>31.528575082222634</v>
+        <v>24.296040623717541</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="8"/>
-        <v>16.553644441058694</v>
+        <v>16.7947763832777</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="9"/>
-        <v>29.087034502204762</v>
+        <v>25.738951092309932</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="10"/>
-        <v>87.176621471075379</v>
+        <v>86.595876739797902</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="11"/>
-        <v>87.176621471075379</v>
+        <v>86.595876739797902</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="12"/>
-        <v>29.087034502204762</v>
+        <v>25.738951092309932</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="13"/>
-        <v>16.553644441058694</v>
+        <v>16.7947763832777</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="14"/>
-        <v>22.820339471631726</v>
+        <v>21.266863737793816</v>
       </c>
       <c r="AB15">
         <v>12.5343</v>
@@ -21256,35 +21256,35 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="7"/>
-        <v>25.492495712980482</v>
+        <v>26.977637231097731</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="8"/>
-        <v>15.240517004233212</v>
+        <v>18.771918912222858</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="9"/>
-        <v>26.211403470825342</v>
+        <v>26.72990000334017</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="10"/>
-        <v>90.435116104374529</v>
+        <v>90.375259727370832</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="11"/>
-        <v>90.435116104374529</v>
+        <v>90.375259727370832</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="12"/>
-        <v>26.211403470825342</v>
+        <v>26.72990000334017</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="13"/>
-        <v>15.240517004233212</v>
+        <v>18.771918912222858</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="14"/>
-        <v>20.725960237529279</v>
+        <v>22.750909457781514</v>
       </c>
       <c r="AB16">
         <v>10.6838</v>
@@ -21336,35 +21336,35 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="7"/>
-        <v>23.524062286953402</v>
+        <v>29.732412542709906</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="8"/>
-        <v>12.603060224198551</v>
+        <v>16.647184988744243</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="9"/>
-        <v>24.061530523727789</v>
+        <v>29.131910034835961</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="10"/>
-        <v>90.889902718555419</v>
+        <v>90.519681934767718</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="11"/>
-        <v>90.889902718555419</v>
+        <v>90.519681934767718</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="12"/>
-        <v>24.061530523727789</v>
+        <v>29.131910034835961</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="13"/>
-        <v>12.603060224198551</v>
+        <v>16.647184988744243</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="14"/>
-        <v>18.33229537396317</v>
+        <v>22.889547511790102</v>
       </c>
       <c r="AB17">
         <v>10.097799999999999</v>
@@ -21412,39 +21412,39 @@
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="7"/>
-        <v>25.622249690995979</v>
+        <v>20.540628973777892</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="8"/>
-        <v>15.08445549770784</v>
+        <v>16.326498623696317</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="9"/>
-        <v>25.310105857542343</v>
+        <v>22.258885185989509</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="10"/>
-        <v>92.396401778633063</v>
+        <v>46.038648974559322</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="11"/>
-        <v>92.396401778633063</v>
+        <v>55.294460739265205</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="12"/>
-        <v>25.310105857542343</v>
+        <v>22.258885185989509</v>
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="13"/>
-        <v>15.08445549770784</v>
+        <v>16.326498623696317</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="14"/>
-        <v>20.197280677625091</v>
+        <v>19.292691904842911</v>
       </c>
       <c r="AB18">
         <v>9.4130400000000005</v>
@@ -21492,39 +21492,39 @@
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="7"/>
-        <v>33.629874132407949</v>
+        <v>25.03974672692323</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="8"/>
-        <v>10.274496415490045</v>
+        <v>14.790588376920999</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="9"/>
-        <v>31.965920477434828</v>
+        <v>24.483574418736488</v>
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="10"/>
-        <v>88.92878956524028</v>
+        <v>43.536833332364289</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="11"/>
-        <v>88.92878956524028</v>
+        <v>52.414856861776059</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="12"/>
-        <v>31.965920477434828</v>
+        <v>24.483574418736488</v>
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="13"/>
-        <v>10.274496415490045</v>
+        <v>14.790588376920999</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="14"/>
-        <v>21.120208446462435</v>
+        <v>19.637081397828744</v>
       </c>
       <c r="AB19">
         <v>8.5562000000000005</v>
@@ -21576,35 +21576,35 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="7"/>
-        <v>24.512101351100803</v>
+        <v>24.844414674816981</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="8"/>
-        <v>14.245589611344045</v>
+        <v>13.647592625090283</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="9"/>
-        <v>26.00286517636761</v>
+        <v>24.772246623600882</v>
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="10"/>
-        <v>94.344816931383491</v>
+        <v>95.297216806581318</v>
       </c>
       <c r="P20">
         <f t="shared" ca="1" si="11"/>
-        <v>94.344816931383491</v>
+        <v>95.297216806581318</v>
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="12"/>
-        <v>26.00286517636761</v>
+        <v>24.772246623600882</v>
       </c>
       <c r="R20">
         <f t="shared" ca="1" si="13"/>
-        <v>14.245589611344045</v>
+        <v>13.647592625090283</v>
       </c>
       <c r="S20">
         <f t="shared" ca="1" si="14"/>
-        <v>20.124227393855826</v>
+        <v>19.209919624345581</v>
       </c>
       <c r="AB20">
         <v>7.9345800000000004</v>
@@ -21652,39 +21652,39 @@
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="7"/>
-        <v>25.974739184945978</v>
+        <v>23.553005174107465</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="8"/>
-        <v>19.167117909755781</v>
+        <v>13.517109086458346</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="9"/>
-        <v>25.980364383230306</v>
+        <v>23.796853464006148</v>
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="10"/>
-        <v>90.503750467150283</v>
+        <v>45.297975968785927</v>
       </c>
       <c r="P21">
         <f t="shared" ca="1" si="11"/>
-        <v>90.503750467150283</v>
+        <v>54.36489361584475</v>
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="12"/>
-        <v>25.980364383230306</v>
+        <v>23.796853464006148</v>
       </c>
       <c r="R21">
         <f t="shared" ca="1" si="13"/>
-        <v>19.167117909755781</v>
+        <v>13.517109086458346</v>
       </c>
       <c r="S21">
         <f t="shared" ca="1" si="14"/>
-        <v>22.573741146493042</v>
+        <v>18.656981275232248</v>
       </c>
       <c r="AB21">
         <v>15.4214</v>
@@ -21736,35 +21736,35 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="7"/>
-        <v>22.503242997124783</v>
+        <v>29.673248723678871</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="8"/>
-        <v>19.338634690717473</v>
+        <v>18.717095203175752</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="9"/>
-        <v>23.198667274345887</v>
+        <v>28.497969671744329</v>
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="10"/>
-        <v>94.748922842168326</v>
+        <v>94.12221143173619</v>
       </c>
       <c r="P22">
         <f t="shared" ca="1" si="11"/>
-        <v>94.748922842168326</v>
+        <v>94.12221143173619</v>
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="12"/>
-        <v>23.198667274345887</v>
+        <v>28.497969671744329</v>
       </c>
       <c r="R22">
         <f t="shared" ca="1" si="13"/>
-        <v>19.338634690717473</v>
+        <v>18.717095203175752</v>
       </c>
       <c r="S22">
         <f t="shared" ca="1" si="14"/>
-        <v>21.268650982531682</v>
+        <v>23.607532437460041</v>
       </c>
       <c r="AB22">
         <v>11.3246</v>
@@ -21812,39 +21812,39 @@
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="7"/>
-        <v>27.978835936763232</v>
+        <v>21.606312128786666</v>
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="8"/>
-        <v>16.552374345472636</v>
+        <v>18.524278372461524</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="9"/>
-        <v>27.022802204279763</v>
+        <v>22.984643637378198</v>
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="10"/>
-        <v>92.741841782295452</v>
+        <v>45.875949719701822</v>
       </c>
       <c r="P23">
         <f t="shared" ca="1" si="11"/>
-        <v>92.741841782295452</v>
+        <v>55.131761484407704</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="12"/>
-        <v>27.022802204279763</v>
+        <v>22.984643637378198</v>
       </c>
       <c r="R23">
         <f t="shared" ca="1" si="13"/>
-        <v>16.552374345472636</v>
+        <v>18.524278372461524</v>
       </c>
       <c r="S23">
         <f t="shared" ca="1" si="14"/>
-        <v>21.7875882748762</v>
+        <v>20.754461004919861</v>
       </c>
       <c r="AB23">
         <v>7.1011600000000001</v>
@@ -21896,35 +21896,35 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="7"/>
-        <v>23.207043685099663</v>
+        <v>27.483418742905489</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="8"/>
-        <v>15.096427487120485</v>
+        <v>20.71529030284762</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="9"/>
-        <v>23.970195388935682</v>
+        <v>26.583663721800033</v>
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="10"/>
-        <v>92.471995593560422</v>
+        <v>92.607262176590794</v>
       </c>
       <c r="P24">
         <f t="shared" ca="1" si="11"/>
-        <v>92.471995593560422</v>
+        <v>92.607262176590794</v>
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="12"/>
-        <v>23.970195388935682</v>
+        <v>26.583663721800033</v>
       </c>
       <c r="R24">
         <f t="shared" ca="1" si="13"/>
-        <v>15.096427487120485</v>
+        <v>20.71529030284762</v>
       </c>
       <c r="S24">
         <f t="shared" ca="1" si="14"/>
-        <v>19.533311438028083</v>
+        <v>23.649477012323828</v>
       </c>
       <c r="AB24">
         <v>11.790699999999999</v>
@@ -21972,39 +21972,39 @@
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="7"/>
-        <v>24.407552885379335</v>
+        <v>27.844125206326009</v>
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="8"/>
-        <v>17.083125420105304</v>
+        <v>19.474879279340399</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="9"/>
-        <v>24.320081386090607</v>
+        <v>27.592032909420816</v>
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="10"/>
-        <v>47.129289132197414</v>
+        <v>94.207115903211161</v>
       </c>
       <c r="P25">
         <f t="shared" ca="1" si="11"/>
-        <v>56.573995014550356</v>
+        <v>94.207115903211161</v>
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="12"/>
-        <v>24.320081386090607</v>
+        <v>27.592032909420816</v>
       </c>
       <c r="R25">
         <f t="shared" ca="1" si="13"/>
-        <v>17.083125420105304</v>
+        <v>19.474879279340399</v>
       </c>
       <c r="S25">
         <f t="shared" ca="1" si="14"/>
-        <v>20.701603403097955</v>
+        <v>23.533456094380607</v>
       </c>
       <c r="AB25">
         <v>7.1720600000000001</v>
@@ -22052,39 +22052,39 @@
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="7"/>
-        <v>26.592403891638881</v>
+        <v>32.588939842286827</v>
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="8"/>
-        <v>15.291077759443521</v>
+        <v>12.774441542397964</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="9"/>
-        <v>26.137939390529226</v>
+        <v>31.589558455713629</v>
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="10"/>
-        <v>46.083081819018801</v>
+        <v>91.935005122360849</v>
       </c>
       <c r="P26">
         <f t="shared" ca="1" si="11"/>
-        <v>55.338893583724683</v>
+        <v>91.935005122360849</v>
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="12"/>
-        <v>26.137939390529226</v>
+        <v>31.589558455713629</v>
       </c>
       <c r="R26">
         <f t="shared" ca="1" si="13"/>
-        <v>15.291077759443521</v>
+        <v>12.774441542397964</v>
       </c>
       <c r="S26">
         <f t="shared" ca="1" si="14"/>
-        <v>20.714508574986375</v>
+        <v>22.181999999055797</v>
       </c>
       <c r="AB26">
         <v>11.055199999999999</v>
@@ -22132,39 +22132,39 @@
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="7"/>
-        <v>22.63781131462844</v>
+        <v>20.04140286628018</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="8"/>
-        <v>12.371485891951234</v>
+        <v>16.201720618556866</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="9"/>
-        <v>23.337836929808596</v>
+        <v>22.351033984166872</v>
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="10"/>
-        <v>88.475238227270992</v>
+        <v>44.192833903096769</v>
       </c>
       <c r="P27">
         <f t="shared" ca="1" si="11"/>
-        <v>88.475238227270992</v>
+        <v>53.070857432508532</v>
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="12"/>
-        <v>23.337836929808596</v>
+        <v>22.351033984166872</v>
       </c>
       <c r="R27">
         <f t="shared" ca="1" si="13"/>
-        <v>12.371485891951234</v>
+        <v>16.201720618556866</v>
       </c>
       <c r="S27">
         <f t="shared" ca="1" si="14"/>
-        <v>17.854661410879913</v>
+        <v>19.276377301361869</v>
       </c>
       <c r="AB27">
         <v>5.6329700000000003</v>
@@ -22212,39 +22212,39 @@
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="7"/>
-        <v>26.558657504378022</v>
+        <v>23.455323184482378</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="8"/>
-        <v>17.464792035564781</v>
+        <v>12.634186534345524</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="9"/>
-        <v>25.914493389464141</v>
+        <v>23.234465344419277</v>
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="10"/>
-        <v>90.459632769749092</v>
+        <v>44.911533440695862</v>
       </c>
       <c r="P28">
         <f t="shared" ca="1" si="11"/>
-        <v>90.459632769749092</v>
+        <v>53.978451087754685</v>
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="12"/>
-        <v>25.914493389464141</v>
+        <v>23.234465344419277</v>
       </c>
       <c r="R28">
         <f t="shared" ca="1" si="13"/>
-        <v>17.464792035564781</v>
+        <v>12.634186534345524</v>
       </c>
       <c r="S28">
         <f t="shared" ca="1" si="14"/>
-        <v>21.689642712514463</v>
+        <v>17.934325939382401</v>
       </c>
       <c r="AB28">
         <v>4.3788200000000002</v>
@@ -22296,35 +22296,35 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="7"/>
-        <v>28.127590415883979</v>
+        <v>24.77785586168158</v>
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="8"/>
-        <v>11.973883633289953</v>
+        <v>15.112027072439044</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="9"/>
-        <v>27.684971010600016</v>
+        <v>24.469177758229122</v>
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="10"/>
-        <v>91.124527115754532</v>
+        <v>91.076865674527227</v>
       </c>
       <c r="P29">
         <f t="shared" ca="1" si="11"/>
-        <v>91.124527115754532</v>
+        <v>91.076865674527227</v>
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="12"/>
-        <v>27.684971010600016</v>
+        <v>24.469177758229122</v>
       </c>
       <c r="R29">
         <f t="shared" ca="1" si="13"/>
-        <v>11.973883633289953</v>
+        <v>15.112027072439044</v>
       </c>
       <c r="S29">
         <f t="shared" ca="1" si="14"/>
-        <v>19.829427321944983</v>
+        <v>19.790602415334085</v>
       </c>
       <c r="AB29">
         <v>7.12798</v>
@@ -22376,35 +22376,35 @@
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="7"/>
-        <v>22.783142049041256</v>
+        <v>26.619187840122468</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="8"/>
-        <v>20.625141346192805</v>
+        <v>10.996984679591822</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="9"/>
-        <v>23.763507841353007</v>
+        <v>26.189185823743802</v>
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="10"/>
-        <v>87.322885627599717</v>
+        <v>86.460776735612825</v>
       </c>
       <c r="P30">
         <f t="shared" ca="1" si="11"/>
-        <v>87.322885627599717</v>
+        <v>86.460776735612825</v>
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="12"/>
-        <v>23.763507841353007</v>
+        <v>26.189185823743802</v>
       </c>
       <c r="R30">
         <f t="shared" ca="1" si="13"/>
-        <v>20.625141346192805</v>
+        <v>10.996984679591822</v>
       </c>
       <c r="S30">
         <f t="shared" ca="1" si="14"/>
-        <v>22.194324593772905</v>
+        <v>18.593085251667812</v>
       </c>
       <c r="AB30">
         <v>3.10764</v>
@@ -22456,35 +22456,35 @@
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="7"/>
-        <v>27.046984976072569</v>
+        <v>29.153239606802373</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="8"/>
-        <v>13.646789583005873</v>
+        <v>14.728821539318091</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="9"/>
-        <v>26.39028954912866</v>
+        <v>28.560428850190661</v>
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="10"/>
-        <v>88.136555721268451</v>
+        <v>88.757132702114163</v>
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="11"/>
-        <v>88.136555721268451</v>
+        <v>88.757132702114163</v>
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="12"/>
-        <v>26.39028954912866</v>
+        <v>28.560428850190661</v>
       </c>
       <c r="R31">
         <f t="shared" ca="1" si="13"/>
-        <v>13.646789583005873</v>
+        <v>14.728821539318091</v>
       </c>
       <c r="S31">
         <f t="shared" ca="1" si="14"/>
-        <v>20.018539566067268</v>
+        <v>21.644625194754376</v>
       </c>
       <c r="AB31">
         <v>11.0318</v>
@@ -22536,35 +22536,35 @@
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="7"/>
-        <v>26.579549053365149</v>
+        <v>20.329509874936363</v>
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="8"/>
-        <v>14.753841207099613</v>
+        <v>8.7474648244060909</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="9"/>
-        <v>26.541697152517855</v>
+        <v>21.975693669987223</v>
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="10"/>
-        <v>89.274029588135974</v>
+        <v>89.294092413167022</v>
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="11"/>
-        <v>89.274029588135974</v>
+        <v>89.294092413167022</v>
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="12"/>
-        <v>26.541697152517855</v>
+        <v>21.975693669987223</v>
       </c>
       <c r="R32">
         <f t="shared" ca="1" si="13"/>
-        <v>14.753841207099613</v>
+        <v>8.7474648244060909</v>
       </c>
       <c r="S32">
         <f t="shared" ca="1" si="14"/>
-        <v>20.647769179808733</v>
+        <v>15.361579247196657</v>
       </c>
       <c r="AB32">
         <v>1.65354</v>
@@ -22631,35 +22631,35 @@
       </c>
       <c r="K34">
         <f ca="1">COUNTIF(K3:K33,"&gt;0")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L34" s="4">
         <f ca="1">AVERAGE(L3:L32)</f>
-        <v>26.398923516113783</v>
+        <v>26.732655762878444</v>
       </c>
       <c r="M34" s="4">
         <f ca="1">AVERAGE(M3:M32)</f>
-        <v>16.683531301314339</v>
+        <v>17.381533859832054</v>
       </c>
       <c r="N34" s="4">
         <f ca="1">AVERAGE(N3:N32)</f>
-        <v>26.422050394024613</v>
+        <v>26.819264162767347</v>
       </c>
       <c r="O34" s="4">
         <f ca="1">AVERAGE(O3:O32)</f>
-        <v>85.901346652646282</v>
+        <v>81.023136083213572</v>
       </c>
       <c r="Q34" s="8">
         <f ca="1">AVERAGE(Q3:Q32)</f>
-        <v>26.422050394024613</v>
+        <v>26.819264162767347</v>
       </c>
       <c r="R34" s="8">
         <f ca="1">AVERAGE(R3:R32)</f>
-        <v>16.683531301314339</v>
+        <v>17.381533859832054</v>
       </c>
       <c r="S34">
         <f ca="1">AVERAGE(S3:S32)</f>
-        <v>21.552790847669474</v>
+        <v>22.100399011299704</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
@@ -22686,27 +22686,27 @@
       </c>
       <c r="L35">
         <f ca="1">_xlfn.STDEV.P(L3:L32)</f>
-        <v>3.6128488203798286</v>
+        <v>3.4092748808747508</v>
       </c>
       <c r="M35">
         <f t="shared" ref="M35:N35" ca="1" si="18">_xlfn.STDEV.P(M3:M32)</f>
-        <v>2.8328034300141529</v>
+        <v>3.704663997251493</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="18"/>
-        <v>2.8834525112984024</v>
+        <v>2.797867479856524</v>
       </c>
       <c r="O35">
         <f t="shared" ref="O35" ca="1" si="19">_xlfn.STDEV.P(O3:O32)</f>
-        <v>19.424174914917423</v>
+        <v>21.807606410371513</v>
       </c>
       <c r="Q35">
         <f ca="1">_xlfn.STDEV.P(Q3:Q32)</f>
-        <v>2.8834525112984024</v>
+        <v>2.797867479856524</v>
       </c>
       <c r="R35">
         <f ca="1">_xlfn.STDEV.P(R3:R32)</f>
-        <v>2.8328034300141529</v>
+        <v>3.704663997251493</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
@@ -35088,7 +35088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I371"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>